<commit_message>
fixes up to recent
</commit_message>
<xml_diff>
--- a/assets/posesaxl.xlsx
+++ b/assets/posesaxl.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jam/go/i9posesa/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F4BE9A-2033-564A-B173-28410A243971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ImageSets" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <sheet name="Transitions" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Exercises!$A$2:$DC$150</definedName>
+    <definedName hidden="true" localSheetId="1" name="_xlnm._FilterDatabase">Exercises!$A$2:$DC$150</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12629" uniqueCount="7197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12636" uniqueCount="7203">
   <si>
     <t>ID</t>
   </si>
@@ -21628,20 +21627,38 @@
     <t>Plank Walkout Half Way</t>
   </si>
   <si>
-    <t>Pushup Down</t>
-  </si>
-  <si>
     <t>Standing T Pose Squat Stance</t>
   </si>
   <si>
     <t>Forearm Plank Hips Up</t>
+  </si>
+  <si>
+    <t>Kneeling on Knee - Both</t>
+  </si>
+  <si>
+    <t>Squat Stance Toes</t>
+  </si>
+  <si>
+    <t>Squat Stance Left High Knee</t>
+  </si>
+  <si>
+    <t>Squat Stance Right High Knee</t>
+  </si>
+  <si>
+    <t>Squat Stance Left High Knee Out</t>
+  </si>
+  <si>
+    <t>Squat Stance Right High Knee Out</t>
+  </si>
+  <si>
+    <t>Downward Walkout</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -21685,12 +21702,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -21707,7 +21724,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -21720,7 +21737,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -22016,10 +22033,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0C6FEDB-7242-034A-A2CD-5F1C567957CE}">
-  <dimension ref="A1:AA258"/>
+  <dimension ref="A1:AA265"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A233" workbookViewId="0">
+      <selection activeCell="B266" sqref="B266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23311,7 +23328,7 @@
       </c>
     </row>
     <row r="17" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C17" t="s">
@@ -23791,7 +23808,7 @@
       </c>
     </row>
     <row r="23" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>151</v>
       </c>
       <c r="C23" t="s">
@@ -24431,7 +24448,7 @@
       </c>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>171</v>
       </c>
       <c r="C31" t="s">
@@ -24911,7 +24928,7 @@
       </c>
     </row>
     <row r="37" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>177</v>
       </c>
       <c r="C37" t="s">
@@ -28271,7 +28288,7 @@
       </c>
     </row>
     <row r="79" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C79" t="s">
@@ -29071,7 +29088,7 @@
       </c>
     </row>
     <row r="89" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="3" t="s">
         <v>168</v>
       </c>
       <c r="C89" t="s">
@@ -29151,7 +29168,7 @@
       </c>
     </row>
     <row r="90" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B90" s="4" t="s">
+      <c r="B90" s="3" t="s">
         <v>169</v>
       </c>
       <c r="C90" t="s">
@@ -29471,7 +29488,7 @@
       </c>
     </row>
     <row r="94" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B94" s="4" t="s">
+      <c r="B94" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C94" t="s">
@@ -29631,7 +29648,7 @@
       </c>
     </row>
     <row r="96" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B96" s="4" t="s">
+      <c r="B96" s="3" t="s">
         <v>544</v>
       </c>
       <c r="C96" t="s">
@@ -30111,7 +30128,7 @@
       </c>
     </row>
     <row r="102" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B102" s="4" t="s">
+      <c r="B102" s="3" t="s">
         <v>546</v>
       </c>
       <c r="C102" t="s">
@@ -30191,7 +30208,7 @@
       </c>
     </row>
     <row r="103" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B103" s="4" t="s">
+      <c r="B103" s="3" t="s">
         <v>549</v>
       </c>
       <c r="C103" t="s">
@@ -30271,7 +30288,7 @@
       </c>
     </row>
     <row r="104" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B104" s="4" t="s">
+      <c r="B104" s="3" t="s">
         <v>550</v>
       </c>
       <c r="C104" t="s">
@@ -30351,7 +30368,7 @@
       </c>
     </row>
     <row r="105" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B105" s="4" t="s">
+      <c r="B105" s="3" t="s">
         <v>548</v>
       </c>
       <c r="C105" t="s">
@@ -31071,7 +31088,7 @@
       </c>
     </row>
     <row r="114" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B114" s="4" t="s">
+      <c r="B114" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C114" t="s">
@@ -31151,7 +31168,7 @@
       </c>
     </row>
     <row r="115" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B115" s="4" t="s">
+      <c r="B115" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C115" t="s">
@@ -31231,7 +31248,7 @@
       </c>
     </row>
     <row r="116" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B116" s="4" t="s">
+      <c r="B116" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C116" t="s">
@@ -31391,7 +31408,7 @@
       </c>
     </row>
     <row r="118" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B118" s="4" t="s">
+      <c r="B118" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C118" t="s">
@@ -31471,7 +31488,7 @@
       </c>
     </row>
     <row r="119" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B119" s="4" t="s">
+      <c r="B119" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C119" t="s">
@@ -31951,7 +31968,7 @@
       </c>
     </row>
     <row r="125" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B125" s="4" t="s">
+      <c r="B125" s="3" t="s">
         <v>86</v>
       </c>
       <c r="C125" t="s">
@@ -34751,7 +34768,7 @@
       </c>
     </row>
     <row r="160" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B160" s="4" t="s">
+      <c r="B160" s="3" t="s">
         <v>112</v>
       </c>
       <c r="C160" t="s">
@@ -35951,7 +35968,7 @@
       </c>
     </row>
     <row r="175" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B175" s="4" t="s">
+      <c r="B175" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C175" t="s">
@@ -36031,7 +36048,7 @@
       </c>
     </row>
     <row r="176" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B176" s="4" t="s">
+      <c r="B176" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C176" t="s">
@@ -38671,7 +38688,7 @@
       </c>
     </row>
     <row r="209" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B209" s="4" t="s">
+      <c r="B209" s="3" t="s">
         <v>214</v>
       </c>
       <c r="C209" t="s">
@@ -38751,7 +38768,7 @@
       </c>
     </row>
     <row r="210" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B210" s="4" t="s">
+      <c r="B210" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C210" t="s">
@@ -38831,7 +38848,7 @@
       </c>
     </row>
     <row r="211" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B211" s="4" t="s">
+      <c r="B211" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C211" t="s">
@@ -38911,7 +38928,7 @@
       </c>
     </row>
     <row r="212" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B212" s="4" t="s">
+      <c r="B212" s="3" t="s">
         <v>44</v>
       </c>
       <c r="C212" t="s">
@@ -41391,7 +41408,7 @@
       </c>
     </row>
     <row r="243" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B243" s="4" t="s">
+      <c r="B243" s="3" t="s">
         <v>7179</v>
       </c>
       <c r="C243" t="s">
@@ -41399,7 +41416,7 @@
       </c>
     </row>
     <row r="244" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B244" s="4" t="s">
+      <c r="B244" s="3" t="s">
         <v>7181</v>
       </c>
       <c r="C244" t="str">
@@ -41408,7 +41425,7 @@
       </c>
     </row>
     <row r="245" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B245" s="4" t="s">
+      <c r="B245" s="3" t="s">
         <v>7182</v>
       </c>
       <c r="C245" t="str">
@@ -41417,7 +41434,7 @@
       </c>
     </row>
     <row r="246" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B246" s="4" t="s">
+      <c r="B246" s="3" t="s">
         <v>7183</v>
       </c>
       <c r="C246" t="str">
@@ -41426,7 +41443,7 @@
       </c>
     </row>
     <row r="247" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B247" s="4" t="s">
+      <c r="B247" s="3" t="s">
         <v>7184</v>
       </c>
       <c r="C247" t="str">
@@ -41435,7 +41452,7 @@
       </c>
     </row>
     <row r="248" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B248" s="4" t="s">
+      <c r="B248" s="3" t="s">
         <v>7185</v>
       </c>
       <c r="C248" t="str">
@@ -41444,7 +41461,7 @@
       </c>
     </row>
     <row r="249" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B249" s="4" t="s">
+      <c r="B249" s="3" t="s">
         <v>7186</v>
       </c>
       <c r="C249" t="str">
@@ -41453,7 +41470,7 @@
       </c>
     </row>
     <row r="250" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B250" s="4" t="s">
+      <c r="B250" s="3" t="s">
         <v>7187</v>
       </c>
       <c r="C250" t="str">
@@ -41462,7 +41479,7 @@
       </c>
     </row>
     <row r="251" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B251" s="4" t="s">
+      <c r="B251" s="3" t="s">
         <v>7188</v>
       </c>
       <c r="C251" t="str">
@@ -41471,16 +41488,16 @@
       </c>
     </row>
     <row r="252" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B252" s="4" t="s">
+      <c r="B252" s="3" t="s">
         <v>7189</v>
       </c>
       <c r="C252" t="str">
-        <f t="shared" ref="C252:C258" si="1">LOWER(SUBSTITUTE(SUBSTITUTE(B252," ","-"),"---","-"))</f>
+        <f t="shared" ref="C252:C265" si="1">LOWER(SUBSTITUTE(SUBSTITUTE(B252," ","-"),"---","-"))</f>
         <v>jumping-jack-half</v>
       </c>
     </row>
     <row r="253" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B253" s="4" t="s">
+      <c r="B253" s="3" t="s">
         <v>7190</v>
       </c>
       <c r="C253" t="str">
@@ -41489,7 +41506,7 @@
       </c>
     </row>
     <row r="254" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B254" s="4" t="s">
+      <c r="B254" s="3" t="s">
         <v>7191</v>
       </c>
       <c r="C254" t="str">
@@ -41498,7 +41515,7 @@
       </c>
     </row>
     <row r="255" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B255" s="4" t="s">
+      <c r="B255" s="3" t="s">
         <v>7192</v>
       </c>
       <c r="C255" t="str">
@@ -41507,7 +41524,7 @@
       </c>
     </row>
     <row r="256" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B256" s="4" t="s">
+      <c r="B256" s="3" t="s">
         <v>7193</v>
       </c>
       <c r="C256" t="str">
@@ -41516,8 +41533,8 @@
       </c>
     </row>
     <row r="257" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B257" s="4" t="s">
-        <v>7195</v>
+      <c r="B257" s="3" t="s">
+        <v>7194</v>
       </c>
       <c r="C257" t="str">
         <f t="shared" si="1"/>
@@ -41525,16 +41542,79 @@
       </c>
     </row>
     <row r="258" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B258" s="4" t="s">
-        <v>7196</v>
+      <c r="B258" s="3" t="s">
+        <v>7195</v>
       </c>
       <c r="C258" t="str">
         <f t="shared" si="1"/>
         <v>forearm-plank-hips-up</v>
       </c>
     </row>
+    <row r="259" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B259" s="3" t="s">
+        <v>7196</v>
+      </c>
+      <c r="C259" t="str">
+        <f t="shared" si="1"/>
+        <v>kneeling-on-knee-both</v>
+      </c>
+    </row>
+    <row r="260" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B260" s="3" t="s">
+        <v>7197</v>
+      </c>
+      <c r="C260" t="str">
+        <f t="shared" si="1"/>
+        <v>squat-stance-toes</v>
+      </c>
+    </row>
+    <row r="261" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B261" s="3" t="s">
+        <v>7198</v>
+      </c>
+      <c r="C261" t="str">
+        <f t="shared" si="1"/>
+        <v>squat-stance-left-high-knee</v>
+      </c>
+    </row>
+    <row r="262" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B262" s="3" t="s">
+        <v>7199</v>
+      </c>
+      <c r="C262" t="str">
+        <f t="shared" si="1"/>
+        <v>squat-stance-right-high-knee</v>
+      </c>
+    </row>
+    <row r="263" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B263" s="3" t="s">
+        <v>7200</v>
+      </c>
+      <c r="C263" t="str">
+        <f t="shared" si="1"/>
+        <v>squat-stance-left-high-knee-out</v>
+      </c>
+    </row>
+    <row r="264" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B264" s="3" t="s">
+        <v>7201</v>
+      </c>
+      <c r="C264" t="str">
+        <f t="shared" si="1"/>
+        <v>squat-stance-right-high-knee-out</v>
+      </c>
+    </row>
+    <row r="265" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B265" s="3" t="s">
+        <v>7202</v>
+      </c>
+      <c r="C265" t="str">
+        <f t="shared" si="1"/>
+        <v>downward-walkout</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D3:AA242">
+  <conditionalFormatting sqref="D3:AA242 D243:D249">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -41546,11 +41626,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B5179E-762C-124B-A240-3A035CE5971A}">
   <dimension ref="A1:DC150"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="G32" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="L43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H42" sqref="H42"/>
+      <selection pane="bottomRight" activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -41668,146 +41748,146 @@
       <c r="F1" t="s">
         <v>380</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3" t="s">
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3" t="s">
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3" t="s">
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3" t="s">
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3" t="s">
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4"/>
+      <c r="AG1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
-      <c r="AJ1" s="3"/>
-      <c r="AK1" s="3"/>
-      <c r="AL1" s="3" t="s">
+      <c r="AH1" s="4"/>
+      <c r="AI1" s="4"/>
+      <c r="AJ1" s="4"/>
+      <c r="AK1" s="4"/>
+      <c r="AL1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
-      <c r="AO1" s="3"/>
-      <c r="AP1" s="3"/>
-      <c r="AQ1" s="3" t="s">
+      <c r="AM1" s="4"/>
+      <c r="AN1" s="4"/>
+      <c r="AO1" s="4"/>
+      <c r="AP1" s="4"/>
+      <c r="AQ1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="AR1" s="3"/>
-      <c r="AS1" s="3"/>
-      <c r="AT1" s="3"/>
-      <c r="AU1" s="3"/>
-      <c r="AV1" s="3" t="s">
+      <c r="AR1" s="4"/>
+      <c r="AS1" s="4"/>
+      <c r="AT1" s="4"/>
+      <c r="AU1" s="4"/>
+      <c r="AV1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="AW1" s="3"/>
-      <c r="AX1" s="3"/>
-      <c r="AY1" s="3"/>
-      <c r="AZ1" s="3"/>
-      <c r="BA1" s="3" t="s">
+      <c r="AW1" s="4"/>
+      <c r="AX1" s="4"/>
+      <c r="AY1" s="4"/>
+      <c r="AZ1" s="4"/>
+      <c r="BA1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="BB1" s="3"/>
-      <c r="BC1" s="3"/>
-      <c r="BD1" s="3"/>
-      <c r="BE1" s="3"/>
-      <c r="BF1" s="3" t="s">
+      <c r="BB1" s="4"/>
+      <c r="BC1" s="4"/>
+      <c r="BD1" s="4"/>
+      <c r="BE1" s="4"/>
+      <c r="BF1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="BG1" s="3"/>
-      <c r="BH1" s="3"/>
-      <c r="BI1" s="3"/>
-      <c r="BJ1" s="3"/>
-      <c r="BK1" s="3" t="s">
+      <c r="BG1" s="4"/>
+      <c r="BH1" s="4"/>
+      <c r="BI1" s="4"/>
+      <c r="BJ1" s="4"/>
+      <c r="BK1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="BL1" s="3"/>
-      <c r="BM1" s="3"/>
-      <c r="BN1" s="3"/>
-      <c r="BO1" s="3"/>
-      <c r="BP1" s="3" t="s">
+      <c r="BL1" s="4"/>
+      <c r="BM1" s="4"/>
+      <c r="BN1" s="4"/>
+      <c r="BO1" s="4"/>
+      <c r="BP1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="BQ1" s="3"/>
-      <c r="BR1" s="3"/>
-      <c r="BS1" s="3"/>
-      <c r="BT1" s="3"/>
-      <c r="BU1" s="3" t="s">
+      <c r="BQ1" s="4"/>
+      <c r="BR1" s="4"/>
+      <c r="BS1" s="4"/>
+      <c r="BT1" s="4"/>
+      <c r="BU1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="BV1" s="3"/>
-      <c r="BW1" s="3"/>
-      <c r="BX1" s="3"/>
-      <c r="BY1" s="3"/>
-      <c r="BZ1" s="3" t="s">
+      <c r="BV1" s="4"/>
+      <c r="BW1" s="4"/>
+      <c r="BX1" s="4"/>
+      <c r="BY1" s="4"/>
+      <c r="BZ1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="CA1" s="3"/>
-      <c r="CB1" s="3"/>
-      <c r="CC1" s="3"/>
-      <c r="CD1" s="3"/>
-      <c r="CE1" s="3" t="s">
+      <c r="CA1" s="4"/>
+      <c r="CB1" s="4"/>
+      <c r="CC1" s="4"/>
+      <c r="CD1" s="4"/>
+      <c r="CE1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="CF1" s="3"/>
-      <c r="CG1" s="3"/>
-      <c r="CH1" s="3"/>
-      <c r="CI1" s="3"/>
-      <c r="CJ1" s="3" t="s">
+      <c r="CF1" s="4"/>
+      <c r="CG1" s="4"/>
+      <c r="CH1" s="4"/>
+      <c r="CI1" s="4"/>
+      <c r="CJ1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="CK1" s="3"/>
-      <c r="CL1" s="3"/>
-      <c r="CM1" s="3"/>
-      <c r="CN1" s="3"/>
-      <c r="CO1" s="3" t="s">
+      <c r="CK1" s="4"/>
+      <c r="CL1" s="4"/>
+      <c r="CM1" s="4"/>
+      <c r="CN1" s="4"/>
+      <c r="CO1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="CP1" s="3"/>
-      <c r="CQ1" s="3"/>
-      <c r="CR1" s="3"/>
-      <c r="CS1" s="3"/>
-      <c r="CT1" s="3" t="s">
+      <c r="CP1" s="4"/>
+      <c r="CQ1" s="4"/>
+      <c r="CR1" s="4"/>
+      <c r="CS1" s="4"/>
+      <c r="CT1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="CU1" s="3"/>
-      <c r="CV1" s="3"/>
-      <c r="CW1" s="3"/>
-      <c r="CX1" s="3"/>
-      <c r="CY1" s="3" t="s">
+      <c r="CU1" s="4"/>
+      <c r="CV1" s="4"/>
+      <c r="CW1" s="4"/>
+      <c r="CX1" s="4"/>
+      <c r="CY1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="CZ1" s="3"/>
-      <c r="DA1" s="3"/>
-      <c r="DB1" s="3"/>
-      <c r="DC1" s="3"/>
+      <c r="CZ1" s="4"/>
+      <c r="DA1" s="4"/>
+      <c r="DB1" s="4"/>
+      <c r="DC1" s="4"/>
     </row>
     <row r="2" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -42282,7 +42362,7 @@
         <v>946</v>
       </c>
       <c r="H5" t="s">
-        <v>7195</v>
+        <v>7194</v>
       </c>
       <c r="I5" t="s">
         <v>381</v>
@@ -42356,7 +42436,7 @@
         <v>381</v>
       </c>
       <c r="H6" t="s">
-        <v>7195</v>
+        <v>7194</v>
       </c>
       <c r="I6" t="s">
         <v>381</v>
@@ -42436,10 +42516,13 @@
         <v>92</v>
       </c>
       <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>381</v>
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="M7" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q7">
+        <v>0.33300000000000002</v>
       </c>
       <c r="V7" t="s">
         <v>381</v>
@@ -42498,10 +42581,13 @@
         <v>93</v>
       </c>
       <c r="L8">
-        <v>1</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>381</v>
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="M8" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q8">
+        <v>0.33300000000000002</v>
       </c>
       <c r="V8" t="s">
         <v>381</v>
@@ -43220,14 +43306,13 @@
         <v>381</v>
       </c>
       <c r="Q18">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="R18" t="s">
         <v>71</v>
       </c>
       <c r="V18">
-        <f>1-Q18-L18</f>
-        <v>0.45000000000000007</v>
+        <v>0.35</v>
       </c>
       <c r="AA18" t="s">
         <v>381</v>
@@ -43304,14 +43389,13 @@
         <v>381</v>
       </c>
       <c r="Q19">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="R19" t="s">
         <v>154</v>
       </c>
       <c r="V19">
-        <f t="shared" ref="V19:V21" si="0">1-Q19-L19</f>
-        <v>0.45000000000000007</v>
+        <v>0.35</v>
       </c>
       <c r="AA19" t="s">
         <v>381</v>
@@ -43394,14 +43478,13 @@
         <v>381</v>
       </c>
       <c r="Q20">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="R20" t="s">
         <v>70</v>
       </c>
       <c r="V20">
-        <f t="shared" si="0"/>
-        <v>0.45000000000000007</v>
+        <v>0.35</v>
       </c>
       <c r="AA20" t="s">
         <v>381</v>
@@ -43478,14 +43561,13 @@
         <v>381</v>
       </c>
       <c r="Q21">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="R21" t="s">
         <v>155</v>
       </c>
       <c r="V21">
-        <f t="shared" si="0"/>
-        <v>0.45000000000000007</v>
+        <v>0.35</v>
       </c>
       <c r="AA21" t="s">
         <v>381</v>
@@ -43861,13 +43943,13 @@
         <v>381</v>
       </c>
       <c r="L26">
-        <v>0.22500000000000001</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="M26" t="s">
         <v>14</v>
       </c>
       <c r="Q26">
-        <v>0.77500000000000002</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="V26" t="s">
         <v>381</v>
@@ -43935,13 +44017,13 @@
         <v>381</v>
       </c>
       <c r="L27">
-        <v>0.22500000000000001</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="M27" t="s">
         <v>15</v>
       </c>
       <c r="Q27">
-        <v>0.77500000000000002</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="V27" t="s">
         <v>381</v>
@@ -44187,7 +44269,6 @@
         <v>541</v>
       </c>
       <c r="AA30">
-        <f>1-AF30-V30-Q30-L30</f>
         <v>0.35</v>
       </c>
       <c r="AB30" t="s">
@@ -44277,7 +44358,6 @@
         <v>542</v>
       </c>
       <c r="AA31">
-        <f>1-AF31-V31-Q31-L31</f>
         <v>0.35</v>
       </c>
       <c r="AB31" t="s">
@@ -44355,7 +44435,7 @@
         <v>1</v>
       </c>
       <c r="O32">
-        <v>0.3</v>
+        <v>0.375</v>
       </c>
       <c r="Q32" t="s">
         <v>381</v>
@@ -44432,7 +44512,7 @@
         <v>1</v>
       </c>
       <c r="O33">
-        <v>0.3</v>
+        <v>0.375</v>
       </c>
       <c r="Q33" t="s">
         <v>381</v>
@@ -44699,7 +44779,7 @@
         <v>381</v>
       </c>
       <c r="L36">
-        <v>0.1</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="M36" t="s">
         <v>199</v>
@@ -44714,7 +44794,7 @@
         <v>381</v>
       </c>
       <c r="Q36">
-        <v>0.1</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="R36" t="s">
         <v>545</v>
@@ -44729,7 +44809,7 @@
         <v>381</v>
       </c>
       <c r="V36">
-        <v>0.1</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="W36" t="s">
         <v>546</v>
@@ -44744,7 +44824,7 @@
         <v>381</v>
       </c>
       <c r="AA36">
-        <v>0.3</v>
+        <v>0.22500000000000006</v>
       </c>
       <c r="AB36" t="s">
         <v>545</v>
@@ -44759,13 +44839,13 @@
         <v>381</v>
       </c>
       <c r="AF36">
-        <v>0.3</v>
+        <v>0.22500000000000006</v>
       </c>
       <c r="AG36" t="s">
         <v>199</v>
       </c>
       <c r="AK36">
-        <v>0.1</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="AP36" t="s">
         <v>381</v>
@@ -44818,7 +44898,7 @@
         <v>381</v>
       </c>
       <c r="L37">
-        <v>0.1</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="M37" t="s">
         <v>205</v>
@@ -44833,7 +44913,7 @@
         <v>381</v>
       </c>
       <c r="Q37">
-        <v>0.1</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="R37" t="s">
         <v>547</v>
@@ -44848,7 +44928,7 @@
         <v>381</v>
       </c>
       <c r="V37">
-        <v>0.1</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="W37" t="s">
         <v>548</v>
@@ -44863,7 +44943,7 @@
         <v>381</v>
       </c>
       <c r="AA37">
-        <v>0.3</v>
+        <v>0.22500000000000006</v>
       </c>
       <c r="AB37" t="s">
         <v>547</v>
@@ -44878,13 +44958,13 @@
         <v>381</v>
       </c>
       <c r="AF37">
-        <v>0.3</v>
+        <v>0.22500000000000006</v>
       </c>
       <c r="AG37" t="s">
         <v>205</v>
       </c>
       <c r="AK37">
-        <v>0.1</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="AP37" t="s">
         <v>381</v>
@@ -44963,7 +45043,7 @@
       <c r="R38" t="s">
         <v>7183</v>
       </c>
-      <c r="V38" s="4">
+      <c r="V38" s="3">
         <v>0.125</v>
       </c>
       <c r="W38" t="s">
@@ -45079,7 +45159,7 @@
       <c r="R39" t="s">
         <v>7184</v>
       </c>
-      <c r="V39" s="4">
+      <c r="V39" s="3">
         <v>0.125</v>
       </c>
       <c r="W39" t="s">
@@ -45201,7 +45281,7 @@
       <c r="R40" t="s">
         <v>7183</v>
       </c>
-      <c r="V40" s="4">
+      <c r="V40" s="3">
         <v>0.1</v>
       </c>
       <c r="W40" t="s">
@@ -45341,7 +45421,7 @@
       <c r="R41" t="s">
         <v>7184</v>
       </c>
-      <c r="V41" s="4">
+      <c r="V41" s="3">
         <v>0.1</v>
       </c>
       <c r="W41" t="s">
@@ -45467,13 +45547,13 @@
         <v>381</v>
       </c>
       <c r="L42">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="M42" t="s">
         <v>195</v>
       </c>
       <c r="Q42">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="V42" t="s">
         <v>381</v>
@@ -45541,13 +45621,13 @@
         <v>381</v>
       </c>
       <c r="L43">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="M43" t="s">
         <v>195</v>
       </c>
       <c r="Q43">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="V43" t="s">
         <v>381</v>
@@ -45618,19 +45698,25 @@
         <v>381</v>
       </c>
       <c r="L44">
-        <v>0.5</v>
+        <v>0.36</v>
       </c>
       <c r="M44" t="s">
+        <v>7189</v>
+      </c>
+      <c r="Q44">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="R44" t="s">
         <v>201</v>
       </c>
-      <c r="Q44">
-        <v>0.5</v>
-      </c>
-      <c r="V44" t="s">
-        <v>381</v>
-      </c>
-      <c r="AA44" t="s">
-        <v>381</v>
+      <c r="V44">
+        <v>0.36</v>
+      </c>
+      <c r="W44" t="s">
+        <v>7189</v>
+      </c>
+      <c r="AA44">
+        <v>0.14000000000000001</v>
       </c>
       <c r="AF44" t="s">
         <v>381</v>
@@ -45695,19 +45781,25 @@
         <v>381</v>
       </c>
       <c r="L45">
-        <v>0.5</v>
+        <v>0.36</v>
       </c>
       <c r="M45" t="s">
+        <v>7190</v>
+      </c>
+      <c r="Q45">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="R45" t="s">
         <v>198</v>
       </c>
-      <c r="Q45">
-        <v>0.5</v>
-      </c>
-      <c r="V45" t="s">
-        <v>381</v>
-      </c>
-      <c r="AA45" t="s">
-        <v>381</v>
+      <c r="V45">
+        <v>0.36</v>
+      </c>
+      <c r="W45" t="s">
+        <v>7190</v>
+      </c>
+      <c r="AA45">
+        <v>0.14000000000000001</v>
       </c>
       <c r="AF45" t="s">
         <v>381</v>
@@ -45772,19 +45864,25 @@
         <v>381</v>
       </c>
       <c r="L46">
-        <v>0.5</v>
+        <v>0.36</v>
       </c>
       <c r="M46" t="s">
+        <v>7189</v>
+      </c>
+      <c r="Q46">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="R46" t="s">
         <v>201</v>
       </c>
-      <c r="Q46">
-        <v>0.5</v>
-      </c>
-      <c r="V46" t="s">
-        <v>381</v>
-      </c>
-      <c r="AA46" t="s">
-        <v>381</v>
+      <c r="V46">
+        <v>0.36</v>
+      </c>
+      <c r="W46" t="s">
+        <v>7189</v>
+      </c>
+      <c r="AA46">
+        <v>0.14000000000000001</v>
       </c>
       <c r="AF46" t="s">
         <v>381</v>
@@ -45843,19 +45941,25 @@
         <v>381</v>
       </c>
       <c r="L47">
-        <v>0.5</v>
+        <v>0.36</v>
       </c>
       <c r="M47" t="s">
+        <v>7190</v>
+      </c>
+      <c r="Q47">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="R47" t="s">
         <v>198</v>
       </c>
-      <c r="Q47">
-        <v>0.5</v>
-      </c>
-      <c r="V47" t="s">
-        <v>381</v>
-      </c>
-      <c r="AA47" t="s">
-        <v>381</v>
+      <c r="V47">
+        <v>0.36</v>
+      </c>
+      <c r="W47" t="s">
+        <v>7190</v>
+      </c>
+      <c r="AA47">
+        <v>0.14000000000000001</v>
       </c>
       <c r="AF47" t="s">
         <v>381</v>
@@ -45920,13 +46024,13 @@
         <v>381</v>
       </c>
       <c r="L48">
-        <v>0.5</v>
+        <v>0.64</v>
       </c>
       <c r="M48" t="s">
         <v>41</v>
       </c>
       <c r="Q48">
-        <v>0.25</v>
+        <v>0.18</v>
       </c>
       <c r="R48" t="s">
         <v>196</v>
@@ -45935,7 +46039,7 @@
         <v>1</v>
       </c>
       <c r="T48">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="V48" t="s">
         <v>381</v>
@@ -45944,7 +46048,7 @@
         <v>41</v>
       </c>
       <c r="AA48">
-        <v>0.25</v>
+        <v>0.18</v>
       </c>
       <c r="AF48" t="s">
         <v>381</v>
@@ -46009,13 +46113,13 @@
         <v>381</v>
       </c>
       <c r="L49">
-        <v>0.5</v>
+        <v>0.64</v>
       </c>
       <c r="M49" t="s">
         <v>41</v>
       </c>
       <c r="Q49">
-        <v>0.25</v>
+        <v>0.18</v>
       </c>
       <c r="R49" t="s">
         <v>72</v>
@@ -46024,7 +46128,7 @@
         <v>1</v>
       </c>
       <c r="T49">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="V49" t="s">
         <v>381</v>
@@ -46033,7 +46137,7 @@
         <v>41</v>
       </c>
       <c r="AA49">
-        <v>0.25</v>
+        <v>0.18</v>
       </c>
       <c r="AF49" t="s">
         <v>381</v>
@@ -46092,13 +46196,13 @@
         <v>381</v>
       </c>
       <c r="L50">
-        <v>0.5</v>
+        <v>0.64</v>
       </c>
       <c r="M50" t="s">
         <v>41</v>
       </c>
       <c r="Q50">
-        <v>0.25</v>
+        <v>0.18</v>
       </c>
       <c r="R50" t="s">
         <v>156</v>
@@ -46107,7 +46211,7 @@
         <v>1</v>
       </c>
       <c r="T50">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="V50" t="s">
         <v>381</v>
@@ -46116,7 +46220,7 @@
         <v>41</v>
       </c>
       <c r="AA50">
-        <v>0.25</v>
+        <v>0.18</v>
       </c>
       <c r="AF50" t="s">
         <v>381</v>
@@ -47521,7 +47625,7 @@
         <v>381</v>
       </c>
       <c r="L64">
-        <v>0.15000000000000002</v>
+        <v>0.17142857142857146</v>
       </c>
       <c r="M64" t="s">
         <v>26</v>
@@ -47536,7 +47640,7 @@
         <v>381</v>
       </c>
       <c r="Q64">
-        <v>0.15000000000000002</v>
+        <v>0.17142857142857146</v>
       </c>
       <c r="R64" t="s">
         <v>129</v>
@@ -47551,7 +47655,7 @@
         <v>381</v>
       </c>
       <c r="V64">
-        <v>0.15000000000000002</v>
+        <v>0.17142857142857146</v>
       </c>
       <c r="W64" t="s">
         <v>131</v>
@@ -47566,7 +47670,7 @@
         <v>381</v>
       </c>
       <c r="AA64">
-        <v>7.5000000000000011E-2</v>
+        <v>8.5714285714285729E-2</v>
       </c>
       <c r="AB64" t="s">
         <v>129</v>
@@ -47581,7 +47685,7 @@
         <v>381</v>
       </c>
       <c r="AF64">
-        <v>7.5000000000000011E-2</v>
+        <v>8.5714285714285729E-2</v>
       </c>
       <c r="AG64" t="s">
         <v>26</v>
@@ -47596,10 +47700,10 @@
         <v>381</v>
       </c>
       <c r="AK64">
-        <v>0.15000000000000002</v>
+        <v>0.17142857142857146</v>
       </c>
       <c r="AL64" t="s">
-        <v>7185</v>
+        <v>168</v>
       </c>
       <c r="AM64" t="s">
         <v>381</v>
@@ -47611,13 +47715,7 @@
         <v>381</v>
       </c>
       <c r="AP64">
-        <v>0.125</v>
-      </c>
-      <c r="AQ64" t="s">
-        <v>168</v>
-      </c>
-      <c r="AU64">
-        <v>0.125</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="AZ64" t="s">
         <v>381</v>
@@ -48695,7 +48793,7 @@
         <v>381</v>
       </c>
       <c r="L75">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="M75" t="s">
         <v>131</v>
@@ -48710,16 +48808,28 @@
         <v>381</v>
       </c>
       <c r="Q75">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="R75" t="s">
         <v>115</v>
       </c>
       <c r="V75">
-        <v>0.3</v>
-      </c>
-      <c r="AA75" t="s">
-        <v>381</v>
+        <v>0.25</v>
+      </c>
+      <c r="W75" t="s">
+        <v>131</v>
+      </c>
+      <c r="X75" t="s">
+        <v>381</v>
+      </c>
+      <c r="Y75" t="s">
+        <v>381</v>
+      </c>
+      <c r="Z75" t="s">
+        <v>381</v>
+      </c>
+      <c r="AA75">
+        <v>0.25</v>
       </c>
       <c r="AF75" t="s">
         <v>381</v>
@@ -48778,7 +48888,7 @@
         <v>381</v>
       </c>
       <c r="L76">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="M76" t="s">
         <v>131</v>
@@ -48793,16 +48903,28 @@
         <v>381</v>
       </c>
       <c r="Q76">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="R76" t="s">
         <v>119</v>
       </c>
       <c r="V76">
-        <v>0.3</v>
-      </c>
-      <c r="AA76" t="s">
-        <v>381</v>
+        <v>0.25</v>
+      </c>
+      <c r="W76" t="s">
+        <v>131</v>
+      </c>
+      <c r="X76" t="s">
+        <v>381</v>
+      </c>
+      <c r="Y76" t="s">
+        <v>381</v>
+      </c>
+      <c r="Z76" t="s">
+        <v>381</v>
+      </c>
+      <c r="AA76">
+        <v>0.25</v>
       </c>
       <c r="AF76" t="s">
         <v>381</v>
@@ -49495,13 +49617,13 @@
         <v>381</v>
       </c>
       <c r="L85">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="M85" t="s">
         <v>195</v>
       </c>
       <c r="Q85">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="V85" t="s">
         <v>381</v>
@@ -49569,13 +49691,13 @@
         <v>381</v>
       </c>
       <c r="L86">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="M86" t="s">
         <v>195</v>
       </c>
       <c r="Q86">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="V86" t="s">
         <v>381</v>
@@ -49646,7 +49768,7 @@
         <v>381</v>
       </c>
       <c r="L87">
-        <v>0.8</v>
+        <v>0.375</v>
       </c>
       <c r="M87" t="s">
         <v>195</v>
@@ -49661,7 +49783,7 @@
         <v>381</v>
       </c>
       <c r="Q87">
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
       <c r="R87" t="s">
         <v>172</v>
@@ -49675,14 +49797,14 @@
       <c r="U87" t="s">
         <v>381</v>
       </c>
-      <c r="V87" t="s">
-        <v>381</v>
+      <c r="V87">
+        <v>0.375</v>
       </c>
       <c r="W87" t="s">
         <v>195</v>
       </c>
-      <c r="AA87" t="s">
-        <v>381</v>
+      <c r="AA87">
+        <v>0.125</v>
       </c>
       <c r="AF87" t="s">
         <v>381</v>
@@ -49744,7 +49866,7 @@
         <v>381</v>
       </c>
       <c r="L88">
-        <v>0.8</v>
+        <v>0.375</v>
       </c>
       <c r="M88" t="s">
         <v>195</v>
@@ -49759,7 +49881,7 @@
         <v>381</v>
       </c>
       <c r="Q88">
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
       <c r="R88" t="s">
         <v>175</v>
@@ -49773,14 +49895,14 @@
       <c r="U88" t="s">
         <v>381</v>
       </c>
-      <c r="V88" t="s">
-        <v>381</v>
+      <c r="V88">
+        <v>0.375</v>
       </c>
       <c r="W88" t="s">
         <v>195</v>
       </c>
-      <c r="AA88" t="s">
-        <v>381</v>
+      <c r="AA88">
+        <v>0.125</v>
       </c>
       <c r="AF88" t="s">
         <v>381</v>
@@ -50802,7 +50924,7 @@
         <v>381</v>
       </c>
       <c r="L101">
-        <v>0.1</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="M101" t="s">
         <v>199</v>
@@ -50817,7 +50939,7 @@
         <v>381</v>
       </c>
       <c r="Q101">
-        <v>0.1</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="R101" t="s">
         <v>545</v>
@@ -50832,7 +50954,7 @@
         <v>381</v>
       </c>
       <c r="V101">
-        <v>0.1</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="W101" t="s">
         <v>549</v>
@@ -50847,7 +50969,7 @@
         <v>381</v>
       </c>
       <c r="AA101">
-        <v>0.3</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="AB101" t="s">
         <v>545</v>
@@ -50862,13 +50984,13 @@
         <v>381</v>
       </c>
       <c r="AF101">
-        <v>0.3</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="AG101" t="s">
         <v>199</v>
       </c>
       <c r="AK101">
-        <v>0.1</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="AP101" t="s">
         <v>381</v>
@@ -50924,7 +51046,7 @@
         <v>381</v>
       </c>
       <c r="L102">
-        <v>0.1</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="M102" t="s">
         <v>205</v>
@@ -50939,7 +51061,7 @@
         <v>381</v>
       </c>
       <c r="Q102">
-        <v>0.1</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="R102" t="s">
         <v>547</v>
@@ -50954,7 +51076,7 @@
         <v>381</v>
       </c>
       <c r="V102">
-        <v>0.1</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="W102" t="s">
         <v>550</v>
@@ -50969,7 +51091,7 @@
         <v>381</v>
       </c>
       <c r="AA102">
-        <v>0.3</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="AB102" t="s">
         <v>547</v>
@@ -50984,13 +51106,13 @@
         <v>381</v>
       </c>
       <c r="AF102">
-        <v>0.3</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="AG102" t="s">
         <v>205</v>
       </c>
       <c r="AK102">
-        <v>0.1</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="AP102" t="s">
         <v>381</v>
@@ -51559,7 +51681,7 @@
         <v>0.25</v>
       </c>
       <c r="R109" t="s">
-        <v>170</v>
+        <v>7185</v>
       </c>
       <c r="S109" t="s">
         <v>381</v>
@@ -51573,8 +51695,8 @@
       <c r="V109">
         <v>0.15</v>
       </c>
-      <c r="W109" t="s">
-        <v>67</v>
+      <c r="W109" s="3" t="s">
+        <v>7198</v>
       </c>
       <c r="AA109">
         <v>0.3</v>
@@ -51657,7 +51779,7 @@
         <v>0.25</v>
       </c>
       <c r="R110" t="s">
-        <v>170</v>
+        <v>7185</v>
       </c>
       <c r="S110" t="s">
         <v>381</v>
@@ -51671,8 +51793,8 @@
       <c r="V110">
         <v>0.15</v>
       </c>
-      <c r="W110" t="s">
-        <v>151</v>
+      <c r="W110" s="3" t="s">
+        <v>7199</v>
       </c>
       <c r="AA110">
         <v>0.3</v>
@@ -51758,7 +51880,7 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="R111" t="s">
-        <v>170</v>
+        <v>7185</v>
       </c>
       <c r="S111" t="s">
         <v>381</v>
@@ -51772,11 +51894,8 @@
       <c r="V111">
         <v>0.125</v>
       </c>
-      <c r="W111" t="s">
-        <v>69</v>
-      </c>
-      <c r="X111" t="s">
-        <v>381</v>
+      <c r="W111" s="3" t="s">
+        <v>7198</v>
       </c>
       <c r="Y111" t="s">
         <v>381</v>
@@ -51785,13 +51904,13 @@
         <v>381</v>
       </c>
       <c r="AA111">
-        <v>0.125</v>
-      </c>
-      <c r="AB111" t="s">
-        <v>67</v>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AB111" s="3" t="s">
+        <v>7200</v>
       </c>
       <c r="AF111">
-        <v>0.25</v>
+        <v>0.21249999999999999</v>
       </c>
       <c r="AK111" t="s">
         <v>381</v>
@@ -51868,7 +51987,7 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="R112" t="s">
-        <v>170</v>
+        <v>7185</v>
       </c>
       <c r="S112" t="s">
         <v>381</v>
@@ -51882,11 +52001,8 @@
       <c r="V112">
         <v>0.125</v>
       </c>
-      <c r="W112" t="s">
-        <v>153</v>
-      </c>
-      <c r="X112" t="s">
-        <v>381</v>
+      <c r="W112" s="3" t="s">
+        <v>7199</v>
       </c>
       <c r="Y112" t="s">
         <v>381</v>
@@ -51895,13 +52011,13 @@
         <v>381</v>
       </c>
       <c r="AA112">
-        <v>0.125</v>
-      </c>
-      <c r="AB112" t="s">
-        <v>151</v>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AB112" s="3" t="s">
+        <v>7201</v>
       </c>
       <c r="AF112">
-        <v>0.25</v>
+        <v>0.21249999999999999</v>
       </c>
       <c r="AK112" t="s">
         <v>381</v>
@@ -52034,7 +52150,7 @@
         <v>1020</v>
       </c>
       <c r="H114" t="s">
-        <v>29</v>
+        <v>7202</v>
       </c>
       <c r="I114" t="s">
         <v>381</v>
@@ -52207,7 +52323,7 @@
         <v>1021</v>
       </c>
       <c r="H115" t="s">
-        <v>29</v>
+        <v>7202</v>
       </c>
       <c r="I115" t="s">
         <v>381</v>
@@ -53038,7 +53154,7 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="R124" t="s">
-        <v>170</v>
+        <v>7185</v>
       </c>
       <c r="S124" t="s">
         <v>381</v>
@@ -53053,7 +53169,7 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="W124" t="s">
-        <v>176</v>
+        <v>7197</v>
       </c>
       <c r="AA124">
         <v>0.17499999999999999</v>
@@ -53465,7 +53581,7 @@
         <v>0.15</v>
       </c>
       <c r="R129" t="s">
-        <v>7194</v>
+        <v>131</v>
       </c>
       <c r="V129">
         <v>0.17499999999999999</v>
@@ -53486,7 +53602,7 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="AB129" t="s">
-        <v>7194</v>
+        <v>131</v>
       </c>
       <c r="AF129">
         <v>0.17499999999999999</v>
@@ -53504,7 +53620,6 @@
         <v>381</v>
       </c>
       <c r="AK129">
-        <f>1-AF129-AA129-V129-Q129-L129</f>
         <v>0.17499999999999996</v>
       </c>
       <c r="AM129" t="s">
@@ -53585,7 +53700,7 @@
         <v>0.15</v>
       </c>
       <c r="R130" t="s">
-        <v>7194</v>
+        <v>131</v>
       </c>
       <c r="V130">
         <v>0.17499999999999999</v>
@@ -53606,7 +53721,7 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="AB130" t="s">
-        <v>7194</v>
+        <v>131</v>
       </c>
       <c r="AF130">
         <v>0.17499999999999999</v>
@@ -53615,7 +53730,6 @@
         <v>36</v>
       </c>
       <c r="AK130">
-        <f>1-AF130-AA130-V130-Q130-L130</f>
         <v>0.17499999999999996</v>
       </c>
     </row>
@@ -54415,7 +54529,7 @@
         <v>1036</v>
       </c>
       <c r="H138" t="s">
-        <v>29</v>
+        <v>7202</v>
       </c>
       <c r="I138" t="s">
         <v>381</v>
@@ -54701,7 +54815,7 @@
         <v>381</v>
       </c>
       <c r="L140">
-        <v>0.14080000000000001</v>
+        <v>0.15533980582524273</v>
       </c>
       <c r="M140" t="s">
         <v>26</v>
@@ -54716,7 +54830,7 @@
         <v>381</v>
       </c>
       <c r="Q140">
-        <v>0.14080000000000001</v>
+        <v>0.15533980582524273</v>
       </c>
       <c r="R140" t="s">
         <v>129</v>
@@ -54731,7 +54845,7 @@
         <v>381</v>
       </c>
       <c r="V140">
-        <v>4.8000000000000001E-2</v>
+        <v>5.8252427184466021E-2</v>
       </c>
       <c r="W140" t="s">
         <v>132</v>
@@ -54746,7 +54860,7 @@
         <v>381</v>
       </c>
       <c r="AA140">
-        <v>0.14080000000000001</v>
+        <v>0.15533980582524273</v>
       </c>
       <c r="AB140" t="s">
         <v>109</v>
@@ -54761,7 +54875,7 @@
         <v>381</v>
       </c>
       <c r="AF140">
-        <v>7.0400000000000004E-2</v>
+        <v>7.7669902912621366E-2</v>
       </c>
       <c r="AG140" t="s">
         <v>132</v>
@@ -54776,7 +54890,7 @@
         <v>381</v>
       </c>
       <c r="AK140">
-        <v>4.8000000000000001E-2</v>
+        <v>5.8252427184466021E-2</v>
       </c>
       <c r="AL140" t="s">
         <v>129</v>
@@ -54791,7 +54905,7 @@
         <v>381</v>
       </c>
       <c r="AP140">
-        <v>7.0400000000000004E-2</v>
+        <v>7.7669902912621366E-2</v>
       </c>
       <c r="AQ140" t="s">
         <v>26</v>
@@ -54806,10 +54920,10 @@
         <v>381</v>
       </c>
       <c r="AU140">
-        <v>0.14080000000000001</v>
+        <v>0.15533980582524273</v>
       </c>
       <c r="AV140" t="s">
-        <v>7185</v>
+        <v>168</v>
       </c>
       <c r="AW140" t="s">
         <v>381</v>
@@ -54821,13 +54935,7 @@
         <v>381</v>
       </c>
       <c r="AZ140">
-        <v>0.1</v>
-      </c>
-      <c r="BA140" t="s">
-        <v>168</v>
-      </c>
-      <c r="BE140">
-        <v>0.1</v>
+        <v>0.10679611650485438</v>
       </c>
       <c r="BJ140" t="s">
         <v>381</v>
@@ -55928,6 +56036,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:DC150" xr:uid="{E9B5179E-762C-124B-A240-3A035CE5971A}"/>
   <mergeCells count="20">
     <mergeCell ref="BK1:BO1"/>
     <mergeCell ref="H1:L1"/>
@@ -55958,8 +56067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899AC92B-5D4B-8E46-9E29-8D79D673E29D}">
   <dimension ref="A1:BC44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -55982,106 +56091,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3" t="s">
+      <c r="I1" s="4"/>
+      <c r="J1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3" t="s">
+      <c r="K1" s="4"/>
+      <c r="L1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3" t="s">
+      <c r="M1" s="4"/>
+      <c r="N1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3" t="s">
+      <c r="O1" s="4"/>
+      <c r="P1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3" t="s">
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3" t="s">
+      <c r="S1" s="4"/>
+      <c r="T1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3" t="s">
+      <c r="U1" s="4"/>
+      <c r="V1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3" t="s">
+      <c r="W1" s="4"/>
+      <c r="X1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3" t="s">
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3" t="s">
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3" t="s">
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3" t="s">
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="3" t="s">
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="AI1" s="3"/>
-      <c r="AJ1" s="3" t="s">
+      <c r="AI1" s="4"/>
+      <c r="AJ1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="AK1" s="3"/>
-      <c r="AL1" s="3" t="s">
+      <c r="AK1" s="4"/>
+      <c r="AL1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="3" t="s">
+      <c r="AM1" s="4"/>
+      <c r="AN1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="AO1" s="3"/>
-      <c r="AP1" s="3" t="s">
+      <c r="AO1" s="4"/>
+      <c r="AP1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="AQ1" s="3"/>
-      <c r="AR1" s="3" t="s">
+      <c r="AQ1" s="4"/>
+      <c r="AR1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="AS1" s="3"/>
-      <c r="AT1" s="3" t="s">
+      <c r="AS1" s="4"/>
+      <c r="AT1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="AU1" s="3"/>
-      <c r="AV1" s="3" t="s">
+      <c r="AU1" s="4"/>
+      <c r="AV1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="AW1" s="3"/>
-      <c r="AX1" s="3" t="s">
+      <c r="AW1" s="4"/>
+      <c r="AX1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="AY1" s="3"/>
-      <c r="AZ1" s="3" t="s">
+      <c r="AY1" s="4"/>
+      <c r="AZ1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="BA1" s="3"/>
-      <c r="BB1" s="3" t="s">
+      <c r="BA1" s="4"/>
+      <c r="BB1" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="BC1" s="3"/>
+      <c r="BC1" s="4"/>
     </row>
     <row r="2" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -56680,7 +56789,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>723</v>
       </c>
@@ -56706,7 +56815,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>409</v>
       </c>
@@ -56726,7 +56835,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>724</v>
       </c>
@@ -56752,7 +56861,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>410</v>
       </c>
@@ -56772,7 +56881,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>725</v>
       </c>
@@ -56798,7 +56907,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>411</v>
       </c>
@@ -56818,7 +56927,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>726</v>
       </c>
@@ -56844,7 +56953,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>412</v>
       </c>
@@ -56864,7 +56973,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>727</v>
       </c>
@@ -56890,7 +56999,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>728</v>
       </c>
@@ -56916,7 +57025,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>414</v>
       </c>
@@ -56936,7 +57045,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>729</v>
       </c>
@@ -56962,7 +57071,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>415</v>
       </c>
@@ -56982,7 +57091,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>730</v>
       </c>
@@ -56999,22 +57108,28 @@
         <v>50</v>
       </c>
       <c r="G30">
-        <v>0.25</v>
+        <v>0.21</v>
       </c>
       <c r="H30" t="s">
         <v>51</v>
       </c>
       <c r="I30">
-        <v>0.5</v>
+        <v>0.37</v>
       </c>
       <c r="J30" t="s">
         <v>50</v>
       </c>
       <c r="K30">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.21</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>7196</v>
+      </c>
+      <c r="M30">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>416</v>
       </c>
@@ -57025,22 +57140,28 @@
         <v>52</v>
       </c>
       <c r="G31">
-        <v>0.25</v>
+        <v>0.21</v>
       </c>
       <c r="H31" t="s">
         <v>53</v>
       </c>
       <c r="I31">
-        <v>0.5</v>
+        <v>0.37</v>
       </c>
       <c r="J31" t="s">
         <v>52</v>
       </c>
       <c r="K31">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.21</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>7196</v>
+      </c>
+      <c r="M31">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>731</v>
       </c>
@@ -57421,7 +57542,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -57868,11 +57989,12 @@
   <dimension ref="A1:I156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" customWidth="1"/>
@@ -59031,7 +59153,7 @@
         <v>609</v>
       </c>
       <c r="E58">
-        <v>2.75</v>
+        <v>2.125</v>
       </c>
       <c r="I58" t="s">
         <v>554</v>
@@ -59211,7 +59333,7 @@
         <v>609</v>
       </c>
       <c r="E67">
-        <v>1.75</v>
+        <v>1.375</v>
       </c>
       <c r="I67" t="s">
         <v>554</v>
@@ -59371,7 +59493,7 @@
         <v>609</v>
       </c>
       <c r="E75">
-        <v>0.3125</v>
+        <v>0.4</v>
       </c>
       <c r="I75" t="s">
         <v>554</v>
@@ -59391,7 +59513,7 @@
         <v>609</v>
       </c>
       <c r="E76">
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="I76" t="s">
         <v>554</v>
@@ -59411,7 +59533,7 @@
         <v>609</v>
       </c>
       <c r="E77">
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="I77" t="s">
         <v>554</v>
@@ -59431,7 +59553,7 @@
         <v>609</v>
       </c>
       <c r="E78">
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="I78" t="s">
         <v>554</v>
@@ -59451,7 +59573,7 @@
         <v>609</v>
       </c>
       <c r="E79">
-        <v>2.5</v>
+        <v>2.85</v>
       </c>
       <c r="I79" t="s">
         <v>554</v>
@@ -59471,7 +59593,7 @@
         <v>609</v>
       </c>
       <c r="E80">
-        <v>2.5</v>
+        <v>2.85</v>
       </c>
       <c r="I80" t="s">
         <v>554</v>
@@ -59811,7 +59933,7 @@
         <v>609</v>
       </c>
       <c r="E97">
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="I97" t="s">
         <v>554</v>
@@ -59851,7 +59973,7 @@
         <v>609</v>
       </c>
       <c r="E99">
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="I99" t="s">
         <v>554</v>
@@ -59871,7 +59993,7 @@
         <v>609</v>
       </c>
       <c r="E100">
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="I100" t="s">
         <v>554</v>
@@ -59891,7 +60013,7 @@
         <v>609</v>
       </c>
       <c r="E101">
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="I101" t="s">
         <v>554</v>
@@ -59911,7 +60033,7 @@
         <v>609</v>
       </c>
       <c r="E102">
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="I102" t="s">
         <v>554</v>
@@ -59971,7 +60093,7 @@
         <v>609</v>
       </c>
       <c r="E105">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="I105" t="s">
         <v>554</v>
@@ -59991,7 +60113,7 @@
         <v>609</v>
       </c>
       <c r="E106">
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="I106" t="s">
         <v>554</v>
@@ -60011,7 +60133,7 @@
         <v>609</v>
       </c>
       <c r="E107">
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="I107" t="s">
         <v>554</v>
@@ -60031,7 +60153,7 @@
         <v>609</v>
       </c>
       <c r="E108">
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="I108" t="s">
         <v>554</v>
@@ -60091,7 +60213,7 @@
         <v>609</v>
       </c>
       <c r="E111">
-        <v>0.3125</v>
+        <v>0.4</v>
       </c>
       <c r="I111" t="s">
         <v>554</v>
@@ -60111,7 +60233,7 @@
         <v>609</v>
       </c>
       <c r="E112">
-        <v>0.625</v>
+        <v>0.8</v>
       </c>
       <c r="I112" t="s">
         <v>554</v>
@@ -60151,7 +60273,7 @@
         <v>609</v>
       </c>
       <c r="E114">
-        <v>2</v>
+        <v>1.6</v>
       </c>
       <c r="I114" t="s">
         <v>554</v>
@@ -60171,7 +60293,7 @@
         <v>609</v>
       </c>
       <c r="E115">
-        <v>1.875</v>
+        <v>1.333</v>
       </c>
       <c r="I115" t="s">
         <v>554</v>
@@ -60191,7 +60313,7 @@
         <v>609</v>
       </c>
       <c r="E116">
-        <v>2</v>
+        <v>1.64</v>
       </c>
       <c r="I116" t="s">
         <v>554</v>
@@ -60331,7 +60453,7 @@
         <v>609</v>
       </c>
       <c r="E123">
-        <v>3.625</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="I123" t="s">
         <v>554</v>
@@ -60411,7 +60533,7 @@
         <v>609</v>
       </c>
       <c r="E127">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="I127" t="s">
         <v>554</v>
@@ -60491,7 +60613,7 @@
         <v>609</v>
       </c>
       <c r="E131">
-        <v>1.75</v>
+        <v>2.35</v>
       </c>
       <c r="I131" t="s">
         <v>554</v>
@@ -60691,7 +60813,7 @@
         <v>609</v>
       </c>
       <c r="E141">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="I141" t="s">
         <v>554</v>
@@ -60771,7 +60893,7 @@
         <v>609</v>
       </c>
       <c r="E145">
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="I145" t="s">
         <v>554</v>
@@ -60811,7 +60933,7 @@
         <v>609</v>
       </c>
       <c r="E147">
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="I147" t="s">
         <v>554</v>
@@ -60831,7 +60953,7 @@
         <v>609</v>
       </c>
       <c r="E148">
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="I148" t="s">
         <v>554</v>
@@ -60851,7 +60973,7 @@
         <v>609</v>
       </c>
       <c r="E149">
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="I149" t="s">
         <v>554</v>
@@ -60871,7 +60993,7 @@
         <v>609</v>
       </c>
       <c r="E150">
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="I150" t="s">
         <v>554</v>
@@ -60891,7 +61013,7 @@
         <v>609</v>
       </c>
       <c r="E151">
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="I151" t="s">
         <v>554</v>
@@ -60911,7 +61033,7 @@
         <v>609</v>
       </c>
       <c r="E152">
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="I152" t="s">
         <v>554</v>
@@ -60931,7 +61053,7 @@
         <v>609</v>
       </c>
       <c r="E153">
-        <v>1.875</v>
+        <v>2.5249999999999999</v>
       </c>
       <c r="I153" t="s">
         <v>554</v>
@@ -61050,36 +61172,36 @@
       <c r="B1" t="s">
         <v>1077</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3" t="s">
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3" t="s">
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3" t="s">
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
complete end of pos file xl
</commit_message>
<xml_diff>
--- a/assets/posesaxl.xlsx
+++ b/assets/posesaxl.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ImageSets" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7213" uniqueCount="7213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12786" uniqueCount="7213">
   <si>
     <t>ID</t>
   </si>
@@ -21399,48 +21399,12 @@
     <t>Start: Standing Up Straight&lt;br&gt;Crouch down so that your hands are on the ground slightly in front of you. Kick both of your legs back and straighten your back to be in pushup position. Bend your arms and squeeze your shoulder blades to go down in a pushup. Push up in an explosive manner so your arms are off the ground and clap your hands together before your hands land on the ground.&lt;br&gt;Return to original pushup position, then jump forward, keeping your hands on the ground so you are in a crouched position. Rise back up to the standing position and jump up around 6 inches off the ground.&lt;br&gt;Once you land, repeat.&lt;br&gt;Primary Body Parts Used: Left Calf, Right Calf, Left Quad, Right Quad, Abs, Lower Back, Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest, Left Hip, Right Hip</t>
   </si>
   <si>
-    <t>Start: Normal Pushup Position&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Pause briefly, then straighten your arms and release your shoulder blades, returning back to pushup position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
-  </si>
-  <si>
-    <t>Start: Normal Pushup Position&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Push up in an explosive manner so your arms are off the ground and clap your hands together before your hands land on the ground.&lt;br&gt;Return back to pushup position and repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
-  </si>
-  <si>
-    <t>Start: Pushup Position with Knees on Ground&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Pause briefly, then straighten your arms and release your shoulder blades, returning back to knee pushup position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
-  </si>
-  <si>
-    <t>Start: Standing Leaned Over Steeply with Hands on Wall&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down, keeping elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly away from the wall. Pause briefly, then straighten your arms and release your shoulder blades, returning back to original position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
-  </si>
-  <si>
-    <t>Start: Standing Leaned Over with Hands on Wall&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down, keeping elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly away from the wall. Pause briefly, then straighten your arms and release your shoulder blades, returning back to original position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
-  </si>
-  <si>
-    <t>Start: Pushup Position with Hands Touching and Legs Apart&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Pause briefly, then straighten your arms and release your shoulder blades, returning back to diamond pushup position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
-  </si>
-  <si>
-    <t>Start: Normal Pushup Position&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Push up in an explosive manner so your arms are off the ground.&lt;br&gt;Return back to pushup position and repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
-  </si>
-  <si>
-    <t>Start: Normal Pushup Position&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. While going down, raise your left leg to your left side by bending at the left knee and hip. Try to touch your left knee to your left elbow. Pause briefly, then straighten your arms and release your shoulder blades, returning back to pushup position.&lt;br&gt;Repeat for right side.&lt;br&gt;Primary Body Parts Used: Left Quad, Right Quad, Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest, Left Hip, Right Hip</t>
-  </si>
-  <si>
-    <t>Start: Normal Pushup Position&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Push up in an explosive manner so your arms are off the ground. Land with your left hand further in front of you and your right hand further behind.&lt;br&gt;Go down in a pushup again and, ensuring elbows are in an "arrow" position and your chest is slightly above the ground. Push up in an explosive manner again and land with your right hand further in front of you and your left hand further behind.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
-  </si>
-  <si>
-    <t>Start: Normal Pushup Position Hands Wide Apart&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Pause briefly, then straighten your arms and release your shoulder blades, returning back to wide pushup position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
-  </si>
-  <si>
-    <t>Start: Normal Pushup Position Hands Close Together&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Pause briefly, then straighten your arms and release your shoulder blades, returning back to narrow pushup position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
-  </si>
-  <si>
     <t>Start: Downward Dog Position&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup-like motion while keeping your hips high in downward dog . Your head should be just slightly above the ground. Pause briefly, then straighten your arms and release your shoulder blades, returning back to downward dog position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
   </si>
   <si>
     <t>Start: Normal Pushup Position Hands Wide Apart&lt;br&gt;Bend your left arm while keeping your right arm straight, to go down so your chest is slightly above the ground and close to your left hand. Pause briefly, then straighten your left arm to push back up to wide pushup position.&lt;br&gt;Bend your right arm while keeping your left arm straight, to go down so your chest is slightly above the ground and close to your right hand. Pause briefly, then straighten your right arm to push back up to wide pushup position.&lt;br&gt;Repeat&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
   </si>
   <si>
-    <t>Start: Downward Dog Position&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup-like motion while keeping your hips high in downward dog . Your head should be just slightly above the ground. Pause briefly, then lower your hips and shift your shoulders forward without straightening your arms or moving your legs, ending in regular pushup down position. Straighten your arms to push back up and raise your hips to re-enter downward dog position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
-  </si>
-  <si>
     <t>Start: Standing Up Straight&lt;br&gt;Jump up around 6 inches (or as high as you are able) off the ground and land your feet slightly in front of where they were originally. Jump back up to the approximate same height and land your feet slightly to the right of where they were originally.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Calf, Right Calf, Left Quad, Right Quad</t>
   </si>
   <si>
@@ -21492,27 +21456,18 @@
     <t>Start: Normal Pushup Position&lt;br&gt;Keeping your hands on the ground, in a "hopping" motion, separate your legs as much as you are able. Pause briefly, then hop again to bring your legs back together in the original pushup position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Abs, Lower Back, Left Tricep, Right Tricep, Left Shoulder, Right Shoulder</t>
   </si>
   <si>
-    <t>Start: Downward Dog Position&lt;br&gt;Keeping your legs on the ground, walk your hands forward and straighten your back until you are in pushup position. Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Pause briefly, then straighten your arms and release your shoulder blades, returning back to pushup position.&lt;br&gt;Walk your hands back while raising your hips until you are back in downward dog position, and repeat.&lt;br&gt;Primary Body Parts Used: Abs, Lower Back, Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Neck, Chest</t>
-  </si>
-  <si>
     <t>Start: Downward Dog Position&lt;br&gt;Keeping your legs on the ground, walk your hands forward and straighten your back until you are in pushup position. Pause briefly, then walk your hands back while raising your hips until you are back in downward dog position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Abs, Lower Back, Left Tricep, Right Tricep, Left Shoulder, Right Shoulder</t>
   </si>
   <si>
     <t>Start: Laying Flat on Stomach with Arms Extended Out in Front&lt;br&gt;Flex your lower back, upper back, and buttocks so that your feet, knees, and arms come off the ground slightly. Bend your elbows and drive them towards your back as far as you are able.&lt;br&gt;Hold this position briefly, then return to the original position and repeat.&lt;br&gt;Primary Body Parts Used: Glutes, Lower Back</t>
   </si>
   <si>
-    <t>Start: Normal Pushup Position &lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping elbows in an "arrow" position (45 degrees from your torso). Go down until your chest touches to floor. Flex your lower back, upper back, and buttocks so that your feet, knees, and arms come off the ground slightly. Bend your elbows and drive them towards your back as far as you are able.&lt;br&gt;Hold briefly, then put your hands and feet back on the ground and push back up so your arms are straight and you are back in original pushup position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Glutes, Lower Back, Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
-  </si>
-  <si>
     <t>Start: Feet on Ground with Knees Bent and Hands Under Shoulders, with Torso Parallel to Ground&lt;br&gt;Keeping your left hand and right foot on the ground for balance and support, raise your right arm and left knee. Touch your left knee with your right hand above your torso and pause briefly.&lt;br&gt;Return to original table position and repeat with your left hand and right knee raised, and right hand and left foot on the ground.&lt;br&gt;Primary Body Parts Used: Left Hamstring, Right Hamstring, Glutes, Abs, Lower Back</t>
   </si>
   <si>
     <t>Start: Feet on Ground with Knees Bent and Hands Under Shoulders, with Torso Parallel to Ground&lt;br&gt;Keeping your left hand and right foot on the ground for balance and support, raise your right arm and left knee. Twist your left leg and bend your left knee to touch your left foot with your right hand above your torso. Pause briefly.&lt;br&gt;Return to original table position and repeat with your left hand and right knee raised, and right hand and left foot on the ground.&lt;br&gt;Primary Body Parts Used: Left Hamstring, Right Hamstring, Glutes, Abs, Lower Back</t>
   </si>
   <si>
-    <t>Start: Normal Pushup Position &lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. While going down, raise your left leg up behind you about 1 foot, while keeping your knee unbent. Pause briefly, then straighten your arms and release your shoulder blades, returning back to pushup position.&lt;br&gt;Repeat for right side.&lt;br&gt;Primary Body Parts Used: Glutes, Lower Back, Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
-  </si>
-  <si>
     <t>Start: Standing with Legs Shoulder-Width Apart&lt;br&gt;Keeping your feet in the same position, squat (bend your knees and hinge at your hips to lower your hips down) so that your quads are approximately parallel to the ground. Pause, then rise back up to original position and flex your calves to end up standing on your toes as high as you can.&lt;br&gt;Repeat, then return to original position and repeat.&lt;br&gt;Primary Body Parts Used: Left Calf, Right Calf, Left Quad, Right Quad, Glutes</t>
   </si>
   <si>
@@ -21540,36 +21495,9 @@
     <t>Start: Standing Up Straight&lt;br&gt;Crouch down so that your hands are on the ground slightly in front of you. Kick both of your legs back and straighten your back to be in regular pushup position. Lower your knees to the ground, entering knee pushup position. Bend your arms and squeeze your shoulder blades to go down in a pushup, then rise back up. Keeping your hands on the ground, use your feet to push and straighten your knees, re-entering regular pushup position.&lt;br&gt;Jump forward, keeping your hands on the ground so you are in a crouched position. Rise back up to the standing position and jump up around 6 inches off the ground.&lt;br&gt;Once you land, repeat.&lt;br&gt;Primary Body Parts Used: Left Calf, Right Calf, Left Quad, Right Quad, Abs, Lower Back, Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest, Left Hip, Right Hip</t>
   </si>
   <si>
-    <t>Start: Downward Dog Position&lt;br&gt;Keeping your legs on the ground, walk your hands forward and straighten your back until you are in pushup position. Lower your knees to the ground, entering knee pushup position. Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground.&lt;br&gt;Straighten your arms and release your shoulder blades, going back to knee pushup position. Keeping your hands on the ground, use your feet to push and straighten your knees, re-entering regular pushup position.&lt;br&gt;Walk your hands back while raising your hips until you are back in downward dog position, and repeat.&lt;br&gt;Primary Body Parts Used: Abs, Lower Back, Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Neck, Chest</t>
-  </si>
-  <si>
-    <t>Start: Pushup Position with Knees on Ground and Hands Touching&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Pause briefly, then straighten your arms and release your shoulder blades, returning back to knee pushup position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
-  </si>
-  <si>
     <t>Start: Standing with Legs Shoulder-Width Apart&lt;br&gt;Crouch down so that your hands are on the ground slightly in front of you. Kick both of your legs back and straighten your back to be in regular pushup position. Lower your knees to the ground, entering knee pushup position. Bend your arms and squeeze your shoulder blades to go down in a pushup, then rise back up. Keeping your hands on the ground, use your feet to push and straighten your knees, re-entering regular pushup position.&lt;br&gt;Jump forward, keeping your hands on the ground so you are in a crouched position. Rise back up to the standing position, then squat down so that your quads are approximately parallel to the ground.&lt;br&gt;Rise back up and repeat.&lt;br&gt;Primary Body Parts Used: Left Quad, Right Quad, Abs, Lower Back, Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest, Left Hip, Right Hip</t>
   </si>
   <si>
-    <t>Start: Pushup Position with Knees on Ground and Hands Wide Apart&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Pause briefly, then straighten your arms and release your shoulder blades, returning back to knee pushup position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
-  </si>
-  <si>
-    <t>Start: Pushup Position with Knees on Ground and Hands Close Together&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Pause briefly, then straighten your arms and release your shoulder blades, returning back to knee pushup position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
-  </si>
-  <si>
-    <t>Start: Standing Leaned Over Steeply with Hands on Wall, Wide Apart&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down, keeping elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly away from the wall. Pause briefly, then straighten your arms and release your shoulder blades, returning back to original position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
-  </si>
-  <si>
-    <t>Start: Standing Leaned Over Steeply with Hands on Wall, Close Together&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down, keeping elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly away from the wall. Pause briefly, then straighten your arms and release your shoulder blades, returning back to original position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
-  </si>
-  <si>
-    <t>Start: Standing Leaned Over with Hands on Wall, Wide Apart&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down, keeping elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly away from the wall. Pause briefly, then straighten your arms and release your shoulder blades, returning back to original position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
-  </si>
-  <si>
-    <t>Start: Standing Leaned Over with Hands on Wall, Close Together&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down, keeping elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly away from the wall. Pause briefly, then straighten your arms and release your shoulder blades, returning back to original position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
-  </si>
-  <si>
-    <t>Start: Normal Pushup Position&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping elbows in an "arrow" position (45 degrees from your torso). Go down until your chest touches to floor. Flex your lower back, upper back, and buttocks so that your feet, knees, and arms come off the ground slightly. Bend your elbows and drive them towards your back as far as you are able.&lt;br&gt;Hold briefly, then put your hands and feet back on the ground and push back up so your arms are straight and you are back in knee pushup position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Glutes, Lower Back, Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
-  </si>
-  <si>
     <t>Start: Standing Up Straight&lt;br&gt;Crouch down so that your hands are on the ground slightly in front of you. Kick both of your legs back and straighten your back to be in regular pushup position. Lower your knees to the ground, entering knee pushup position. Bend your arms and squeeze your shoulder blades to go down in a pushup, then rise back up. Keeping your hands on the ground, use your feet to push and straighten your knees, re-entering regular pushup position.&lt;br&gt;Jump forward, keeping your hands on the ground so you are in a crouched position. Rise back up to the standing position and jump up, raising your knees and tucking them into your chest (or as high as you can raise them)&lt;br&gt;Once you land, repeat.&lt;br&gt;Primary Body Parts Used: Left Calf, Right Calf, Left Quad, Right Quad, Abs, Lower Back, Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest, Left Hip, Right Hip</t>
   </si>
   <si>
@@ -21660,28 +21588,100 @@
     <t>Non-Pushup Step Burpees</t>
   </si>
   <si>
+    <t>66427ff2fe756517596a03f6</t>
+  </si>
+  <si>
+    <t>66427ff2fe756517596a03f5</t>
+  </si>
+  <si>
+    <t>6642808be58eff8b7586550a</t>
+  </si>
+  <si>
+    <t>6642808be58eff8b7586550b</t>
+  </si>
+  <si>
+    <t>664280a1e58eff8b7586550c</t>
+  </si>
+  <si>
+    <t>664280a1e58eff8b7586550d</t>
+  </si>
+  <si>
+    <t>Start: Normal Pushup Position&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Pause briefly, then straighten your arms and release your shoulder blades, returning back to pushup position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
+  </si>
+  <si>
+    <t>Start: Normal Pushup Position&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Push up in an explosive manner so your arms are off the ground and clap your hands together before your hands land on the ground.&lt;br&gt;Return back to pushup position and repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
+  </si>
+  <si>
+    <t>Start: Pushup Position with Knees on Ground&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Pause briefly, then straighten your arms and release your shoulder blades, returning back to knee pushup position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
+  </si>
+  <si>
+    <t>Start: Standing Leaned Over Steeply with Hands on Wall&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly away from the wall. Pause briefly, then straighten your arms and release your shoulder blades, returning back to original position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
+  </si>
+  <si>
+    <t>Start: Standing Leaned Over with Hands on Wall&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly away from the wall. Pause briefly, then straighten your arms and release your shoulder blades, returning back to original position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
+  </si>
+  <si>
+    <t>Start: Pushup Position with Hands Touching and Legs Apart&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Pause briefly, then straighten your arms and release your shoulder blades, returning back to diamond pushup position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
+  </si>
+  <si>
+    <t>Start: Normal Pushup Position&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Push up in an explosive manner so your arms are off the ground.&lt;br&gt;Return back to pushup position and repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
+  </si>
+  <si>
+    <t>Start: Normal Pushup Position&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. While going down, raise your left leg to your left side by bending at the left knee and hip. Try to touch your left knee to your left elbow. Pause briefly, then straighten your arms and release your shoulder blades, returning back to pushup position.&lt;br&gt;Repeat for right side.&lt;br&gt;Primary Body Parts Used: Left Quad, Right Quad, Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest, Left Hip, Right Hip</t>
+  </si>
+  <si>
+    <t>Start: Normal Pushup Position&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Push up in an explosive manner so your arms are off the ground. Land with your left hand further in front of you and your right hand further behind.&lt;br&gt;Go down in a pushup again and, ensuring elbows are in an "arrow" position and your chest is slightly above the ground. Push up in an explosive manner again and land with your right hand further in front of you and your left hand further behind.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
+  </si>
+  <si>
+    <t>Start: Normal Pushup Position Hands Wide Apart&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Pause briefly, then straighten your arms and release your shoulder blades, returning back to wide pushup position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
+  </si>
+  <si>
+    <t>Start: Normal Pushup Position Hands Close Together&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Pause briefly, then straighten your arms and release your shoulder blades, returning back to narrow pushup position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
+  </si>
+  <si>
+    <t>Start: Downward Dog Position&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup-like motion while keeping your abs right and hips high in downward dog . Your head should be just slightly above the ground. Pause briefly, then lower your hips and shift your shoulders forward without straightening your arms or moving your legs, ending in regular pushup down position. Straighten your arms to push back up and raise your hips to re-enter downward dog position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
+  </si>
+  <si>
+    <t>Start: Downward Dog Position&lt;br&gt;Keeping your legs on the ground, walk your hands forward and straighten your back until you are in pushup position. Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Pause briefly, then straighten your arms and release your shoulder blades, returning back to pushup position.&lt;br&gt;Walk your hands back while raising your hips until you are back in downward dog position, and repeat.&lt;br&gt;Primary Body Parts Used: Abs, Lower Back, Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Neck, Chest</t>
+  </si>
+  <si>
+    <t>Start: Normal Pushup Position &lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Go down until your chest touches to floor. Flex your lower back, upper back, and buttocks so that your feet, knees, and arms come off the ground slightly. Bend your elbows and drive them towards your back as far as you are able.&lt;br&gt;Hold briefly, then put your hands and feet back on the ground and push back up so your arms are straight and you are back in original pushup position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Glutes, Lower Back, Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
+  </si>
+  <si>
+    <t>Start: Normal Pushup Position &lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. While going down, raise your left leg up behind you about 1 foot, while keeping your knee unbent. Pause briefly, then straighten your arms and release your shoulder blades, returning back to pushup position.&lt;br&gt;Repeat for right side.&lt;br&gt;Primary Body Parts Used: Glutes, Lower Back, Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
+  </si>
+  <si>
+    <t>Start: Downward Dog Position&lt;br&gt;Keeping your legs on the ground, walk your hands forward and straighten your back until you are in pushup position. Lower your knees to the ground, entering knee pushup position. Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground.&lt;br&gt;Straighten your arms and release your shoulder blades, going back to knee pushup position. Keeping your hands on the ground, use your feet to push and straighten your knees, re-entering regular pushup position.&lt;br&gt;Walk your hands back while raising your hips until you are back in downward dog position, and repeat.&lt;br&gt;Primary Body Parts Used: Abs, Lower Back, Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Neck, Chest</t>
+  </si>
+  <si>
+    <t>Start: Pushup Position with Knees on Ground and Hands Touching&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Pause briefly, then straighten your arms and release your shoulder blades, returning back to knee pushup position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
+  </si>
+  <si>
+    <t>Start: Pushup Position with Knees on Ground and Hands Wide Apart&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Pause briefly, then straighten your arms and release your shoulder blades, returning back to knee pushup position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
+  </si>
+  <si>
+    <t>Start: Pushup Position with Knees on Ground and Hands Close Together&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly above the ground. Pause briefly, then straighten your arms and release your shoulder blades, returning back to knee pushup position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
+  </si>
+  <si>
+    <t>Start: Standing Leaned Over Steeply with Hands on Wall, Wide Apart&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly away from the wall. Pause briefly, then straighten your arms and release your shoulder blades, returning back to original position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
+  </si>
+  <si>
+    <t>Start: Standing Leaned Over Steeply with Hands on Wall, Close Together&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly away from the wall. Pause briefly, then straighten your arms and release your shoulder blades, returning back to original position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
+  </si>
+  <si>
+    <t>Start: Standing Leaned Over with Hands on Wall, Wide Apart&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly away from the wall. Pause briefly, then straighten your arms and release your shoulder blades, returning back to original position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
+  </si>
+  <si>
+    <t>Start: Standing Leaned Over with Hands on Wall, Close Together&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Your chest should be just slightly away from the wall. Pause briefly, then straighten your arms and release your shoulder blades, returning back to original position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
+  </si>
+  <si>
+    <t>Start: Normal Pushup Position&lt;br&gt;Bend your arms and squeeze your shoulder blades to go down in a pushup, keeping your abs tight and elbows in an "arrow" position (45 degrees from your torso). Go down until your chest touches to floor. Flex your lower back, upper back, and buttocks so that your feet, knees, and arms come off the ground slightly. Bend your elbows and drive them towards your back as far as you are able.&lt;br&gt;Hold briefly, then put your hands and feet back on the ground and push back up so your arms are straight and you are back in knee pushup position.&lt;br&gt;Repeat.&lt;br&gt;Primary Body Parts Used: Glutes, Lower Back, Left Tricep, Right Tricep, Left Shoulder, Right Shoulder, Chest</t>
+  </si>
+  <si>
+    <t>Start: Standing Up Straight&lt;br&gt;Crouch down so that your hands are on the ground slightly in front of you. Step your right leg, then left leg back so that you are in pushup position. Lower your knees to the ground, entering knee pushup position. Bend your arms and squeeze your shoulder blades to go down in a pushup, then rise back up. Keeping your hands on the ground, use your feet to push and straighten your knees, re-entering regular pushup position.&lt;br&gt;Step your left leg forward, then right leg while keeping your hands on the ground, so you are in a crouched position. Rise back up to the standing position and repeat.&lt;br&gt;Primary Body Parts Used: Left Quad, Right Quad, Abs, Lower Back, Left Tricep, Right Tricep, Left Shoulder, Right Shoulder</t>
+  </si>
+  <si>
     <t>Start: Standing Up Straight&lt;br&gt;Crouch down so that your hands are on the ground slightly in front of you. Step your right leg, then left leg back so that you are in pushup position.&lt;br&gt;Step your left leg forward, then right leg while keeping your hands on the ground, so you are in a crouched position. Rise back up to the standing position and repeat.&lt;br&gt;Primary Body Parts Used: Left Quad, Right Quad, Abs, Lower Back</t>
-  </si>
-  <si>
-    <t>Start: Standing Up Straight&lt;br&gt;Crouch down so that your hands are on the ground slightly in front of you. Step your right leg, then left leg back so that you are in pushup position. Lower your knees to the ground, entering knee pushup position. Bend your arms and squeeze your shoulder blades to go down in a pushup, then rise back up. Keeping your hands on the ground, use your feet to push and straighten your knees, re-entering regular pushup position.&lt;br&gt;Step your left leg forward, then right leg while keeping your hands on the ground, so you are in a crouched position. Rise back up to the standing position and repeat.&lt;br&gt;Primary Body Parts Used: Left Quad, Right Quad, Abs, Lower Back, Left Tricep, Right Tricep, Left Shoulder, Right Shoulder</t>
-  </si>
-  <si>
-    <t>66427ff2fe756517596a03f6</t>
-  </si>
-  <si>
-    <t>66427ff2fe756517596a03f5</t>
-  </si>
-  <si>
-    <t>6642808be58eff8b7586550a</t>
-  </si>
-  <si>
-    <t>6642808be58eff8b7586550b</t>
-  </si>
-  <si>
-    <t>664280a1e58eff8b7586550c</t>
-  </si>
-  <si>
-    <t>664280a1e58eff8b7586550d</t>
   </si>
 </sst>
 </file>
@@ -41439,15 +41439,15 @@
     </row>
     <row r="243" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B243" s="3" t="s">
-        <v>7179</v>
+        <v>7155</v>
       </c>
       <c r="C243" t="s">
-        <v>7180</v>
+        <v>7156</v>
       </c>
     </row>
     <row r="244" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B244" s="3" t="s">
-        <v>7181</v>
+        <v>7157</v>
       </c>
       <c r="C244" t="str">
         <f>LOWER(SUBSTITUTE(B244," ","-"))</f>
@@ -41456,7 +41456,7 @@
     </row>
     <row r="245" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B245" s="3" t="s">
-        <v>7182</v>
+        <v>7158</v>
       </c>
       <c r="C245" t="str">
         <f>LOWER(SUBSTITUTE(B245," ","-"))</f>
@@ -41465,7 +41465,7 @@
     </row>
     <row r="246" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B246" s="3" t="s">
-        <v>7183</v>
+        <v>7159</v>
       </c>
       <c r="C246" t="str">
         <f t="shared" ref="C246:C248" si="0">LOWER(SUBSTITUTE(B246," ","-"))</f>
@@ -41474,7 +41474,7 @@
     </row>
     <row r="247" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B247" s="3" t="s">
-        <v>7184</v>
+        <v>7160</v>
       </c>
       <c r="C247" t="str">
         <f t="shared" si="0"/>
@@ -41483,7 +41483,7 @@
     </row>
     <row r="248" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B248" s="3" t="s">
-        <v>7185</v>
+        <v>7161</v>
       </c>
       <c r="C248" t="str">
         <f t="shared" si="0"/>
@@ -41492,7 +41492,7 @@
     </row>
     <row r="249" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B249" s="3" t="s">
-        <v>7186</v>
+        <v>7162</v>
       </c>
       <c r="C249" t="str">
         <f>LOWER(SUBSTITUTE(SUBSTITUTE(B249," ","-"),"---","-"))</f>
@@ -41501,7 +41501,7 @@
     </row>
     <row r="250" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B250" s="3" t="s">
-        <v>7187</v>
+        <v>7163</v>
       </c>
       <c r="C250" t="str">
         <f>LOWER(SUBSTITUTE(SUBSTITUTE(B250," ","-"),"---","-"))</f>
@@ -41510,7 +41510,7 @@
     </row>
     <row r="251" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B251" s="3" t="s">
-        <v>7188</v>
+        <v>7164</v>
       </c>
       <c r="C251" t="str">
         <f>LOWER(SUBSTITUTE(SUBSTITUTE(B251," ","-"),"---","-"))</f>
@@ -41519,7 +41519,7 @@
     </row>
     <row r="252" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B252" s="3" t="s">
-        <v>7189</v>
+        <v>7165</v>
       </c>
       <c r="C252" t="str">
         <f t="shared" ref="C252:C265" si="1">LOWER(SUBSTITUTE(SUBSTITUTE(B252," ","-"),"---","-"))</f>
@@ -41528,7 +41528,7 @@
     </row>
     <row r="253" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B253" s="3" t="s">
-        <v>7190</v>
+        <v>7166</v>
       </c>
       <c r="C253" t="str">
         <f t="shared" si="1"/>
@@ -41537,7 +41537,7 @@
     </row>
     <row r="254" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B254" s="3" t="s">
-        <v>7191</v>
+        <v>7167</v>
       </c>
       <c r="C254" t="str">
         <f t="shared" si="1"/>
@@ -41546,7 +41546,7 @@
     </row>
     <row r="255" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B255" s="3" t="s">
-        <v>7192</v>
+        <v>7168</v>
       </c>
       <c r="C255" t="str">
         <f t="shared" si="1"/>
@@ -41555,7 +41555,7 @@
     </row>
     <row r="256" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B256" s="3" t="s">
-        <v>7193</v>
+        <v>7169</v>
       </c>
       <c r="C256" t="str">
         <f t="shared" si="1"/>
@@ -41564,7 +41564,7 @@
     </row>
     <row r="257" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B257" s="3" t="s">
-        <v>7194</v>
+        <v>7170</v>
       </c>
       <c r="C257" t="str">
         <f t="shared" si="1"/>
@@ -41573,7 +41573,7 @@
     </row>
     <row r="258" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B258" s="3" t="s">
-        <v>7195</v>
+        <v>7171</v>
       </c>
       <c r="C258" t="str">
         <f t="shared" si="1"/>
@@ -41582,7 +41582,7 @@
     </row>
     <row r="259" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B259" s="3" t="s">
-        <v>7196</v>
+        <v>7172</v>
       </c>
       <c r="C259" t="str">
         <f t="shared" si="1"/>
@@ -41591,7 +41591,7 @@
     </row>
     <row r="260" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B260" s="3" t="s">
-        <v>7197</v>
+        <v>7173</v>
       </c>
       <c r="C260" t="str">
         <f t="shared" si="1"/>
@@ -41600,7 +41600,7 @@
     </row>
     <row r="261" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B261" s="3" t="s">
-        <v>7198</v>
+        <v>7174</v>
       </c>
       <c r="C261" t="str">
         <f t="shared" si="1"/>
@@ -41609,7 +41609,7 @@
     </row>
     <row r="262" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B262" s="3" t="s">
-        <v>7199</v>
+        <v>7175</v>
       </c>
       <c r="C262" t="str">
         <f t="shared" si="1"/>
@@ -41618,7 +41618,7 @@
     </row>
     <row r="263" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B263" s="3" t="s">
-        <v>7200</v>
+        <v>7176</v>
       </c>
       <c r="C263" t="str">
         <f t="shared" si="1"/>
@@ -41627,7 +41627,7 @@
     </row>
     <row r="264" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B264" s="3" t="s">
-        <v>7201</v>
+        <v>7177</v>
       </c>
       <c r="C264" t="str">
         <f t="shared" si="1"/>
@@ -41636,7 +41636,7 @@
     </row>
     <row r="265" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B265" s="3" t="s">
-        <v>7202</v>
+        <v>7178</v>
       </c>
       <c r="C265" t="str">
         <f t="shared" si="1"/>
@@ -41656,125 +41656,125 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B5179E-762C-124B-A240-3A035CE5971A}">
   <dimension ref="A1:DC152"/>
   <sheetViews>
-    <sheetView tabSelected="true" zoomScaleNormal="100" workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="C124" xSplit="2" ySplit="2"/>
-      <selection activeCell="C1" pane="topRight" sqref="C1"/>
-      <selection activeCell="A3" pane="bottomLeft" sqref="A3"/>
-      <selection activeCell="B151" pane="bottomRight" sqref="B151"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C124" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B151" sqref="B151"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="true" max="1" min="1" width="23.5"/>
-    <col bestFit="true" customWidth="true" max="2" min="2" width="31"/>
-    <col customWidth="true" max="3" min="3" width="16"/>
-    <col customWidth="true" max="4" min="4" width="18"/>
-    <col bestFit="true" customWidth="true" max="5" min="5" width="17.875"/>
-    <col bestFit="true" customWidth="true" max="6" min="6" width="25"/>
-    <col bestFit="true" customWidth="true" max="7" min="7" width="24.875"/>
-    <col bestFit="true" customWidth="true" max="8" min="8" width="41"/>
-    <col bestFit="true" customWidth="true" max="9" min="9" width="12.5"/>
-    <col bestFit="true" customWidth="true" max="10" min="10" width="14.875"/>
-    <col bestFit="true" customWidth="true" max="11" min="11" width="8.875"/>
-    <col bestFit="true" customWidth="true" max="12" min="12" width="11.875"/>
-    <col bestFit="true" customWidth="true" max="13" min="13" width="41.625"/>
-    <col bestFit="true" customWidth="true" max="14" min="14" width="12.5"/>
-    <col bestFit="true" customWidth="true" max="15" min="15" width="14.875"/>
-    <col bestFit="true" customWidth="true" max="16" min="16" width="8.875"/>
-    <col bestFit="true" customWidth="true" max="17" min="17" width="11.875"/>
-    <col bestFit="true" customWidth="true" max="18" min="18" width="40"/>
-    <col bestFit="true" customWidth="true" max="19" min="19" width="12.5"/>
-    <col bestFit="true" customWidth="true" max="20" min="20" width="14.875"/>
-    <col bestFit="true" customWidth="true" max="21" min="21" width="8.875"/>
-    <col bestFit="true" customWidth="true" max="22" min="22" width="11.875"/>
-    <col bestFit="true" customWidth="true" max="23" min="23" width="37.375"/>
-    <col bestFit="true" customWidth="true" max="24" min="24" width="12.5"/>
-    <col bestFit="true" customWidth="true" max="25" min="25" width="14.875"/>
-    <col bestFit="true" customWidth="true" max="26" min="26" width="8.875"/>
-    <col bestFit="true" customWidth="true" max="27" min="27" width="11.875"/>
-    <col bestFit="true" customWidth="true" max="28" min="28" width="28.375"/>
-    <col bestFit="true" customWidth="true" max="29" min="29" width="12.5"/>
-    <col bestFit="true" customWidth="true" max="30" min="30" width="14.875"/>
-    <col bestFit="true" customWidth="true" max="31" min="31" width="8.875"/>
-    <col bestFit="true" customWidth="true" max="32" min="32" width="11.875"/>
-    <col bestFit="true" customWidth="true" max="33" min="33" width="37.375"/>
-    <col bestFit="true" customWidth="true" max="34" min="34" width="12.5"/>
-    <col bestFit="true" customWidth="true" max="35" min="35" width="14.875"/>
-    <col bestFit="true" customWidth="true" max="36" min="36" width="8.875"/>
-    <col bestFit="true" customWidth="true" max="37" min="37" width="11.875"/>
-    <col bestFit="true" customWidth="true" max="38" min="38" width="30.375"/>
-    <col bestFit="true" customWidth="true" max="39" min="39" width="12.5"/>
-    <col bestFit="true" customWidth="true" max="40" min="40" width="14.875"/>
-    <col bestFit="true" customWidth="true" max="41" min="41" width="8.875"/>
-    <col bestFit="true" customWidth="true" max="42" min="42" width="11.875"/>
-    <col bestFit="true" customWidth="true" max="43" min="43" width="37.375"/>
-    <col bestFit="true" customWidth="true" max="44" min="44" width="12.5"/>
-    <col bestFit="true" customWidth="true" max="45" min="45" width="14.875"/>
-    <col bestFit="true" customWidth="true" max="46" min="46" width="8.875"/>
-    <col bestFit="true" customWidth="true" max="47" min="47" width="11.875"/>
-    <col bestFit="true" customWidth="true" max="48" min="48" width="25"/>
-    <col bestFit="true" customWidth="true" max="49" min="49" width="12.5"/>
-    <col bestFit="true" customWidth="true" max="50" min="50" width="14.875"/>
-    <col bestFit="true" customWidth="true" max="51" min="51" width="8.875"/>
-    <col bestFit="true" customWidth="true" max="52" min="52" width="11.875"/>
-    <col bestFit="true" customWidth="true" max="53" min="53" width="28.875"/>
-    <col bestFit="true" customWidth="true" max="54" min="54" width="12.5"/>
-    <col bestFit="true" customWidth="true" max="55" min="55" width="14.875"/>
-    <col bestFit="true" customWidth="true" max="56" min="56" width="8.875"/>
-    <col bestFit="true" customWidth="true" max="57" min="57" width="11.875"/>
-    <col bestFit="true" customWidth="true" max="58" min="58" width="25"/>
-    <col bestFit="true" customWidth="true" max="59" min="59" width="12.5"/>
-    <col bestFit="true" customWidth="true" max="60" min="60" width="14.875"/>
-    <col bestFit="true" customWidth="true" max="61" min="61" width="8.875"/>
-    <col bestFit="true" customWidth="true" max="62" min="62" width="11.875"/>
-    <col bestFit="true" customWidth="true" max="63" min="63" width="26.375"/>
-    <col bestFit="true" customWidth="true" max="64" min="64" width="12.5"/>
-    <col bestFit="true" customWidth="true" max="65" min="65" width="14.875"/>
-    <col bestFit="true" customWidth="true" max="66" min="66" width="8.875"/>
-    <col bestFit="true" customWidth="true" max="67" min="67" width="11.875"/>
-    <col bestFit="true" customWidth="true" max="68" min="68" width="13.875"/>
-    <col bestFit="true" customWidth="true" max="69" min="69" width="12.5"/>
-    <col bestFit="true" customWidth="true" max="70" min="70" width="14.875"/>
-    <col bestFit="true" customWidth="true" max="71" min="71" width="8.875"/>
-    <col bestFit="true" customWidth="true" max="72" min="72" width="11.875"/>
-    <col bestFit="true" customWidth="true" max="73" min="73" width="13.875"/>
-    <col bestFit="true" customWidth="true" max="74" min="74" width="12.5"/>
-    <col bestFit="true" customWidth="true" max="75" min="75" width="14.875"/>
-    <col bestFit="true" customWidth="true" max="76" min="76" width="8.875"/>
-    <col bestFit="true" customWidth="true" max="77" min="77" width="11.875"/>
-    <col bestFit="true" customWidth="true" max="78" min="78" width="13.875"/>
-    <col bestFit="true" customWidth="true" max="79" min="79" width="12.5"/>
-    <col bestFit="true" customWidth="true" max="80" min="80" width="14.875"/>
-    <col bestFit="true" customWidth="true" max="81" min="81" width="8.875"/>
-    <col bestFit="true" customWidth="true" max="82" min="82" width="11.875"/>
-    <col bestFit="true" customWidth="true" max="83" min="83" width="13.875"/>
-    <col bestFit="true" customWidth="true" max="84" min="84" width="12.5"/>
-    <col bestFit="true" customWidth="true" max="85" min="85" width="14.875"/>
-    <col bestFit="true" customWidth="true" max="86" min="86" width="8.875"/>
-    <col bestFit="true" customWidth="true" max="87" min="87" width="11.875"/>
-    <col bestFit="true" customWidth="true" max="88" min="88" width="13.875"/>
-    <col bestFit="true" customWidth="true" max="89" min="89" width="12.5"/>
-    <col bestFit="true" customWidth="true" max="90" min="90" width="14.875"/>
-    <col bestFit="true" customWidth="true" max="91" min="91" width="8.875"/>
-    <col bestFit="true" customWidth="true" max="92" min="92" width="11.875"/>
-    <col bestFit="true" customWidth="true" max="93" min="93" width="13.875"/>
-    <col bestFit="true" customWidth="true" max="94" min="94" width="12.5"/>
-    <col bestFit="true" customWidth="true" max="95" min="95" width="14.875"/>
-    <col bestFit="true" customWidth="true" max="96" min="96" width="8.875"/>
-    <col bestFit="true" customWidth="true" max="97" min="97" width="11.875"/>
-    <col bestFit="true" customWidth="true" max="98" min="98" width="13.875"/>
-    <col bestFit="true" customWidth="true" max="99" min="99" width="12.5"/>
-    <col bestFit="true" customWidth="true" max="100" min="100" width="14.875"/>
-    <col bestFit="true" customWidth="true" max="101" min="101" width="8.875"/>
-    <col bestFit="true" customWidth="true" max="102" min="102" width="11.875"/>
-    <col bestFit="true" customWidth="true" max="103" min="103" width="13.875"/>
-    <col bestFit="true" customWidth="true" max="104" min="104" width="12.5"/>
-    <col bestFit="true" customWidth="true" max="105" min="105" width="14.875"/>
-    <col bestFit="true" customWidth="true" max="106" min="106" width="8.875"/>
-    <col bestFit="true" customWidth="true" max="107" min="107" width="11.875"/>
+    <col min="1" max="1" width="23.5" customWidth="1"/>
+    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="41.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="40" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="37.375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="37.375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="30.375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="37.375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="25" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="28.875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="25" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:107">
+    <row r="1" spans="1:107" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
         <v>380</v>
       </c>
@@ -41919,7 +41919,7 @@
       <c r="DB1" s="4"/>
       <c r="DC1" s="4"/>
     </row>
-    <row r="2" spans="1:107">
+    <row r="2" spans="1:107" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -42242,7 +42242,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="1:107">
+    <row r="3" spans="1:107" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>610</v>
       </c>
@@ -42307,7 +42307,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="4" spans="1:107">
+    <row r="4" spans="1:107" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>427</v>
       </c>
@@ -42369,7 +42369,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="5" spans="1:107">
+    <row r="5" spans="1:107" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>611</v>
       </c>
@@ -42392,7 +42392,7 @@
         <v>946</v>
       </c>
       <c r="H5" t="s">
-        <v>7194</v>
+        <v>7170</v>
       </c>
       <c r="I5" t="s">
         <v>381</v>
@@ -42446,7 +42446,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="6" spans="1:107">
+    <row r="6" spans="1:107" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>428</v>
       </c>
@@ -42466,7 +42466,7 @@
         <v>381</v>
       </c>
       <c r="H6" t="s">
-        <v>7194</v>
+        <v>7170</v>
       </c>
       <c r="I6" t="s">
         <v>381</v>
@@ -42520,7 +42520,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="7" spans="1:107">
+    <row r="7" spans="1:107" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>612</v>
       </c>
@@ -42588,7 +42588,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="8" spans="1:107">
+    <row r="8" spans="1:107" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>429</v>
       </c>
@@ -42653,7 +42653,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="9" spans="1:107">
+    <row r="9" spans="1:107" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>613</v>
       </c>
@@ -42730,7 +42730,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="10" spans="1:107">
+    <row r="10" spans="1:107" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>614</v>
       </c>
@@ -42807,7 +42807,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="11" spans="1:107">
+    <row r="11" spans="1:107" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>431</v>
       </c>
@@ -42881,7 +42881,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="12" spans="1:107">
+    <row r="12" spans="1:107" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>615</v>
       </c>
@@ -42958,7 +42958,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="13" spans="1:107">
+    <row r="13" spans="1:107" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>432</v>
       </c>
@@ -43032,7 +43032,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="14" spans="1:107">
+    <row r="14" spans="1:107" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>616</v>
       </c>
@@ -43097,7 +43097,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="15" spans="1:107">
+    <row r="15" spans="1:107" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>433</v>
       </c>
@@ -43159,7 +43159,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="16" spans="1:107">
+    <row r="16" spans="1:107" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>617</v>
       </c>
@@ -43224,7 +43224,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="17" spans="1:72">
+    <row r="17" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>434</v>
       </c>
@@ -43286,7 +43286,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="18" spans="1:72">
+    <row r="18" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>618</v>
       </c>
@@ -43375,7 +43375,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="19" spans="1:72">
+    <row r="19" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>435</v>
       </c>
@@ -43458,7 +43458,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="20" spans="1:72">
+    <row r="20" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>619</v>
       </c>
@@ -43547,7 +43547,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="21" spans="1:72">
+    <row r="21" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>436</v>
       </c>
@@ -43630,7 +43630,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="22" spans="1:72">
+    <row r="22" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>620</v>
       </c>
@@ -43707,7 +43707,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="23" spans="1:72">
+    <row r="23" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>621</v>
       </c>
@@ -43784,7 +43784,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="24" spans="1:72">
+    <row r="24" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>622</v>
       </c>
@@ -43861,7 +43861,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="25" spans="1:72">
+    <row r="25" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>623</v>
       </c>
@@ -43938,7 +43938,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="26" spans="1:72">
+    <row r="26" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>624</v>
       </c>
@@ -44015,7 +44015,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="27" spans="1:72">
+    <row r="27" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>441</v>
       </c>
@@ -44089,7 +44089,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="28" spans="1:72">
+    <row r="28" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>625</v>
       </c>
@@ -44166,7 +44166,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="29" spans="1:72">
+    <row r="29" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>442</v>
       </c>
@@ -44237,7 +44237,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="30" spans="1:72">
+    <row r="30" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>626</v>
       </c>
@@ -44290,7 +44290,7 @@
         <v>0.125</v>
       </c>
       <c r="R30" t="s">
-        <v>7183</v>
+        <v>7159</v>
       </c>
       <c r="V30">
         <v>0.17499999999999999</v>
@@ -44302,7 +44302,7 @@
         <v>0.35</v>
       </c>
       <c r="AB30" t="s">
-        <v>7183</v>
+        <v>7159</v>
       </c>
       <c r="AF30">
         <v>0.2</v>
@@ -44332,7 +44332,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="31" spans="1:72">
+    <row r="31" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>443</v>
       </c>
@@ -44379,7 +44379,7 @@
         <v>0.125</v>
       </c>
       <c r="R31" t="s">
-        <v>7184</v>
+        <v>7160</v>
       </c>
       <c r="V31">
         <v>0.17499999999999999</v>
@@ -44391,7 +44391,7 @@
         <v>0.35</v>
       </c>
       <c r="AB31" t="s">
-        <v>7184</v>
+        <v>7160</v>
       </c>
       <c r="AF31">
         <v>0.2</v>
@@ -44421,7 +44421,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="32" spans="1:72">
+    <row r="32" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>627</v>
       </c>
@@ -44504,7 +44504,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="33" spans="1:77">
+    <row r="33" spans="1:77" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>444</v>
       </c>
@@ -44581,7 +44581,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="34" spans="1:77">
+    <row r="34" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>628</v>
       </c>
@@ -44682,7 +44682,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="35" spans="1:77">
+    <row r="35" spans="1:77" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>445</v>
       </c>
@@ -44777,7 +44777,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="36" spans="1:77">
+    <row r="36" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>629</v>
       </c>
@@ -44899,7 +44899,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="37" spans="1:77">
+    <row r="37" spans="1:77" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>446</v>
       </c>
@@ -45018,7 +45018,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="38" spans="1:77">
+    <row r="38" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>630</v>
       </c>
@@ -45071,7 +45071,7 @@
         <v>0.13125000000000001</v>
       </c>
       <c r="R38" t="s">
-        <v>7183</v>
+        <v>7159</v>
       </c>
       <c r="V38" s="3">
         <v>0.125</v>
@@ -45113,7 +45113,7 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="AL38" t="s">
-        <v>7183</v>
+        <v>7159</v>
       </c>
       <c r="AP38">
         <v>0.13750000000000001</v>
@@ -45140,7 +45140,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="39" spans="1:77">
+    <row r="39" spans="1:77" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>447</v>
       </c>
@@ -45187,7 +45187,7 @@
         <v>0.13125000000000001</v>
       </c>
       <c r="R39" t="s">
-        <v>7184</v>
+        <v>7160</v>
       </c>
       <c r="V39" s="3">
         <v>0.125</v>
@@ -45229,7 +45229,7 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="AL39" t="s">
-        <v>7184</v>
+        <v>7160</v>
       </c>
       <c r="AP39">
         <v>0.13750000000000001</v>
@@ -45256,7 +45256,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="40" spans="1:77">
+    <row r="40" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>631</v>
       </c>
@@ -45309,7 +45309,7 @@
         <v>0.1</v>
       </c>
       <c r="R40" t="s">
-        <v>7183</v>
+        <v>7159</v>
       </c>
       <c r="V40" s="3">
         <v>0.1</v>
@@ -45381,7 +45381,7 @@
         <v>0.16</v>
       </c>
       <c r="AV40" t="s">
-        <v>7183</v>
+        <v>7159</v>
       </c>
       <c r="AZ40">
         <v>0.1</v>
@@ -45402,7 +45402,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="41" spans="1:77">
+    <row r="41" spans="1:77" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>448</v>
       </c>
@@ -45449,7 +45449,7 @@
         <v>0.1</v>
       </c>
       <c r="R41" t="s">
-        <v>7184</v>
+        <v>7160</v>
       </c>
       <c r="V41" s="3">
         <v>0.1</v>
@@ -45521,7 +45521,7 @@
         <v>0.16</v>
       </c>
       <c r="AV41" t="s">
-        <v>7184</v>
+        <v>7160</v>
       </c>
       <c r="AZ41">
         <v>0.1</v>
@@ -45542,7 +45542,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="42" spans="1:77">
+    <row r="42" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>632</v>
       </c>
@@ -45619,7 +45619,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="43" spans="1:77">
+    <row r="43" spans="1:77" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>449</v>
       </c>
@@ -45693,7 +45693,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="44" spans="1:77">
+    <row r="44" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>633</v>
       </c>
@@ -45731,7 +45731,7 @@
         <v>0.36</v>
       </c>
       <c r="M44" t="s">
-        <v>7189</v>
+        <v>7165</v>
       </c>
       <c r="Q44">
         <v>0.14000000000000001</v>
@@ -45743,7 +45743,7 @@
         <v>0.36</v>
       </c>
       <c r="W44" t="s">
-        <v>7189</v>
+        <v>7165</v>
       </c>
       <c r="AA44">
         <v>0.14000000000000001</v>
@@ -45776,7 +45776,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="45" spans="1:77">
+    <row r="45" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>634</v>
       </c>
@@ -45814,7 +45814,7 @@
         <v>0.36</v>
       </c>
       <c r="M45" t="s">
-        <v>7190</v>
+        <v>7166</v>
       </c>
       <c r="Q45">
         <v>0.14000000000000001</v>
@@ -45826,7 +45826,7 @@
         <v>0.36</v>
       </c>
       <c r="W45" t="s">
-        <v>7190</v>
+        <v>7166</v>
       </c>
       <c r="AA45">
         <v>0.14000000000000001</v>
@@ -45859,7 +45859,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="46" spans="1:77">
+    <row r="46" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>635</v>
       </c>
@@ -45897,7 +45897,7 @@
         <v>0.36</v>
       </c>
       <c r="M46" t="s">
-        <v>7189</v>
+        <v>7165</v>
       </c>
       <c r="Q46">
         <v>0.14000000000000001</v>
@@ -45909,7 +45909,7 @@
         <v>0.36</v>
       </c>
       <c r="W46" t="s">
-        <v>7189</v>
+        <v>7165</v>
       </c>
       <c r="AA46">
         <v>0.14000000000000001</v>
@@ -45942,7 +45942,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="47" spans="1:77">
+    <row r="47" spans="1:77" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>452</v>
       </c>
@@ -45974,7 +45974,7 @@
         <v>0.36</v>
       </c>
       <c r="M47" t="s">
-        <v>7190</v>
+        <v>7166</v>
       </c>
       <c r="Q47">
         <v>0.14000000000000001</v>
@@ -45986,7 +45986,7 @@
         <v>0.36</v>
       </c>
       <c r="W47" t="s">
-        <v>7190</v>
+        <v>7166</v>
       </c>
       <c r="AA47">
         <v>0.14000000000000001</v>
@@ -46019,7 +46019,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="48" spans="1:77">
+    <row r="48" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>636</v>
       </c>
@@ -46108,7 +46108,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="49" spans="1:72">
+    <row r="49" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>637</v>
       </c>
@@ -46197,7 +46197,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="50" spans="1:72">
+    <row r="50" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>454</v>
       </c>
@@ -46280,7 +46280,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="51" spans="1:72">
+    <row r="51" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>638</v>
       </c>
@@ -46303,7 +46303,7 @@
         <v>973</v>
       </c>
       <c r="H51" t="s">
-        <v>7185</v>
+        <v>7161</v>
       </c>
       <c r="I51" t="s">
         <v>381</v>
@@ -46357,7 +46357,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="52" spans="1:72">
+    <row r="52" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>639</v>
       </c>
@@ -46380,7 +46380,7 @@
         <v>974</v>
       </c>
       <c r="H52" t="s">
-        <v>7185</v>
+        <v>7161</v>
       </c>
       <c r="I52" t="s">
         <v>381</v>
@@ -46443,7 +46443,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="53" spans="1:72">
+    <row r="53" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>640</v>
       </c>
@@ -46466,7 +46466,7 @@
         <v>975</v>
       </c>
       <c r="H53" t="s">
-        <v>7192</v>
+        <v>7168</v>
       </c>
       <c r="I53" t="s">
         <v>381</v>
@@ -46520,7 +46520,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="54" spans="1:72">
+    <row r="54" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>641</v>
       </c>
@@ -46597,7 +46597,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="55" spans="1:72">
+    <row r="55" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>642</v>
       </c>
@@ -46620,7 +46620,7 @@
         <v>977</v>
       </c>
       <c r="H55" t="s">
-        <v>7185</v>
+        <v>7161</v>
       </c>
       <c r="I55" t="s">
         <v>381</v>
@@ -46674,7 +46674,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="56" spans="1:72">
+    <row r="56" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>643</v>
       </c>
@@ -46697,7 +46697,7 @@
         <v>978</v>
       </c>
       <c r="H56" t="s">
-        <v>7185</v>
+        <v>7161</v>
       </c>
       <c r="I56" t="s">
         <v>381</v>
@@ -46775,7 +46775,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="57" spans="1:72">
+    <row r="57" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>644</v>
       </c>
@@ -46798,7 +46798,7 @@
         <v>979</v>
       </c>
       <c r="H57" t="s">
-        <v>7185</v>
+        <v>7161</v>
       </c>
       <c r="I57" t="s">
         <v>381</v>
@@ -46900,7 +46900,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="58" spans="1:72">
+    <row r="58" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>645</v>
       </c>
@@ -46923,7 +46923,7 @@
         <v>980</v>
       </c>
       <c r="H58" t="s">
-        <v>7185</v>
+        <v>7161</v>
       </c>
       <c r="I58" t="s">
         <v>381</v>
@@ -46986,7 +46986,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="59" spans="1:72">
+    <row r="59" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>462</v>
       </c>
@@ -47003,7 +47003,7 @@
         <v>381</v>
       </c>
       <c r="H59" t="s">
-        <v>7192</v>
+        <v>7168</v>
       </c>
       <c r="I59" t="s">
         <v>381</v>
@@ -47066,7 +47066,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="60" spans="1:72">
+    <row r="60" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>646</v>
       </c>
@@ -47209,7 +47209,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="61" spans="1:72">
+    <row r="61" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>647</v>
       </c>
@@ -47358,7 +47358,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="62" spans="1:72">
+    <row r="62" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>648</v>
       </c>
@@ -47477,7 +47477,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="63" spans="1:72">
+    <row r="63" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>649</v>
       </c>
@@ -47620,7 +47620,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="64" spans="1:72">
+    <row r="64" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>650</v>
       </c>
@@ -47643,7 +47643,7 @@
         <v>985</v>
       </c>
       <c r="H64" t="s">
-        <v>7185</v>
+        <v>7161</v>
       </c>
       <c r="I64" t="s">
         <v>381</v>
@@ -47763,7 +47763,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="65" spans="1:72">
+    <row r="65" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>651</v>
       </c>
@@ -47906,7 +47906,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="66" spans="1:72">
+    <row r="66" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>652</v>
       </c>
@@ -48049,7 +48049,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="67" spans="1:72">
+    <row r="67" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>653</v>
       </c>
@@ -48216,7 +48216,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="68" spans="1:72">
+    <row r="68" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>654</v>
       </c>
@@ -48293,7 +48293,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="69" spans="1:72">
+    <row r="69" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>655</v>
       </c>
@@ -48385,7 +48385,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="70" spans="1:72">
+    <row r="70" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>656</v>
       </c>
@@ -48462,7 +48462,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="71" spans="1:72">
+    <row r="71" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>657</v>
       </c>
@@ -48539,7 +48539,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="72" spans="1:72">
+    <row r="72" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>658</v>
       </c>
@@ -48616,7 +48616,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="73" spans="1:72">
+    <row r="73" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>659</v>
       </c>
@@ -48693,7 +48693,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="74" spans="1:72">
+    <row r="74" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>660</v>
       </c>
@@ -48788,7 +48788,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="75" spans="1:72">
+    <row r="75" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>661</v>
       </c>
@@ -48889,7 +48889,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="76" spans="1:72">
+    <row r="76" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>478</v>
       </c>
@@ -48984,7 +48984,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="77" spans="1:72">
+    <row r="77" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>662</v>
       </c>
@@ -49061,7 +49061,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="78" spans="1:72">
+    <row r="78" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>479</v>
       </c>
@@ -49132,7 +49132,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="79" spans="1:72">
+    <row r="79" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>663</v>
       </c>
@@ -49209,7 +49209,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="80" spans="1:72">
+    <row r="80" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>664</v>
       </c>
@@ -49286,7 +49286,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="81" spans="1:72">
+    <row r="81" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>665</v>
       </c>
@@ -49363,7 +49363,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="82" spans="1:72">
+    <row r="82" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>666</v>
       </c>
@@ -49440,7 +49440,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="83" spans="1:72">
+    <row r="83" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>483</v>
       </c>
@@ -49511,7 +49511,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="84" spans="1:72">
+    <row r="84" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>667</v>
       </c>
@@ -49612,7 +49612,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="85" spans="1:72">
+    <row r="85" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>668</v>
       </c>
@@ -49689,7 +49689,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="86" spans="1:72">
+    <row r="86" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>485</v>
       </c>
@@ -49763,7 +49763,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="87" spans="1:72">
+    <row r="87" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>669</v>
       </c>
@@ -49864,7 +49864,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="88" spans="1:72">
+    <row r="88" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>486</v>
       </c>
@@ -49962,7 +49962,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="89" spans="1:72">
+    <row r="89" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>670</v>
       </c>
@@ -50039,7 +50039,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="90" spans="1:72">
+    <row r="90" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>487</v>
       </c>
@@ -50113,7 +50113,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="91" spans="1:72">
+    <row r="91" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>671</v>
       </c>
@@ -50136,7 +50136,7 @@
         <v>1006</v>
       </c>
       <c r="H91" t="s">
-        <v>7188</v>
+        <v>7164</v>
       </c>
       <c r="L91">
         <v>0.35</v>
@@ -50190,7 +50190,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="92" spans="1:72">
+    <row r="92" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>488</v>
       </c>
@@ -50210,7 +50210,7 @@
         <v>381</v>
       </c>
       <c r="H92" t="s">
-        <v>7188</v>
+        <v>7164</v>
       </c>
       <c r="L92">
         <v>0.35</v>
@@ -50264,7 +50264,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="93" spans="1:72">
+    <row r="93" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>672</v>
       </c>
@@ -50302,7 +50302,7 @@
         <v>0.3</v>
       </c>
       <c r="M93" t="s">
-        <v>7188</v>
+        <v>7164</v>
       </c>
       <c r="Q93">
         <v>0.2</v>
@@ -50314,7 +50314,7 @@
         <v>0.3</v>
       </c>
       <c r="W93" t="s">
-        <v>7188</v>
+        <v>7164</v>
       </c>
       <c r="AA93">
         <v>0.2</v>
@@ -50347,7 +50347,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="94" spans="1:72">
+    <row r="94" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>673</v>
       </c>
@@ -50370,7 +50370,7 @@
         <v>1008</v>
       </c>
       <c r="H94" t="s">
-        <v>7188</v>
+        <v>7164</v>
       </c>
       <c r="L94">
         <v>0.35</v>
@@ -50424,7 +50424,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="95" spans="1:72">
+    <row r="95" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>490</v>
       </c>
@@ -50444,7 +50444,7 @@
         <v>381</v>
       </c>
       <c r="H95" t="s">
-        <v>7188</v>
+        <v>7164</v>
       </c>
       <c r="L95">
         <v>0.35</v>
@@ -50498,7 +50498,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="96" spans="1:72">
+    <row r="96" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>674</v>
       </c>
@@ -50596,7 +50596,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="97" spans="1:72">
+    <row r="97" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>491</v>
       </c>
@@ -50691,7 +50691,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="98" spans="1:72">
+    <row r="98" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>675</v>
       </c>
@@ -50768,7 +50768,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="99" spans="1:72">
+    <row r="99" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>676</v>
       </c>
@@ -50845,7 +50845,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="100" spans="1:72">
+    <row r="100" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>493</v>
       </c>
@@ -50919,7 +50919,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="101" spans="1:72">
+    <row r="101" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>677</v>
       </c>
@@ -51044,7 +51044,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="102" spans="1:72">
+    <row r="102" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>494</v>
       </c>
@@ -51166,7 +51166,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="103" spans="1:72">
+    <row r="103" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>678</v>
       </c>
@@ -51267,7 +51267,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="104" spans="1:72">
+    <row r="104" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>679</v>
       </c>
@@ -51344,7 +51344,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="105" spans="1:72">
+    <row r="105" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>680</v>
       </c>
@@ -51421,7 +51421,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="106" spans="1:72">
+    <row r="106" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>497</v>
       </c>
@@ -51495,7 +51495,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="107" spans="1:72">
+    <row r="107" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>681</v>
       </c>
@@ -51533,7 +51533,7 @@
         <v>0.3</v>
       </c>
       <c r="M107" t="s">
-        <v>7186</v>
+        <v>7162</v>
       </c>
       <c r="Q107">
         <v>0.2</v>
@@ -51545,7 +51545,7 @@
         <v>0.3</v>
       </c>
       <c r="W107" t="s">
-        <v>7186</v>
+        <v>7162</v>
       </c>
       <c r="AA107">
         <v>0.2</v>
@@ -51578,7 +51578,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="108" spans="1:72">
+    <row r="108" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>498</v>
       </c>
@@ -51613,7 +51613,7 @@
         <v>0.3</v>
       </c>
       <c r="M108" t="s">
-        <v>7187</v>
+        <v>7163</v>
       </c>
       <c r="Q108">
         <v>0.2</v>
@@ -51625,7 +51625,7 @@
         <v>0.3</v>
       </c>
       <c r="W108" t="s">
-        <v>7187</v>
+        <v>7163</v>
       </c>
       <c r="AA108">
         <v>0.2</v>
@@ -51658,7 +51658,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="109" spans="1:72">
+    <row r="109" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>682</v>
       </c>
@@ -51681,7 +51681,7 @@
         <v>1017</v>
       </c>
       <c r="H109" t="s">
-        <v>7185</v>
+        <v>7161</v>
       </c>
       <c r="I109" t="s">
         <v>381</v>
@@ -51711,7 +51711,7 @@
         <v>0.25</v>
       </c>
       <c r="R109" t="s">
-        <v>7185</v>
+        <v>7161</v>
       </c>
       <c r="S109" t="s">
         <v>381</v>
@@ -51726,7 +51726,7 @@
         <v>0.15</v>
       </c>
       <c r="W109" s="3" t="s">
-        <v>7198</v>
+        <v>7174</v>
       </c>
       <c r="AA109">
         <v>0.3</v>
@@ -51759,7 +51759,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="110" spans="1:72">
+    <row r="110" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>499</v>
       </c>
@@ -51779,7 +51779,7 @@
         <v>381</v>
       </c>
       <c r="H110" t="s">
-        <v>7185</v>
+        <v>7161</v>
       </c>
       <c r="I110" t="s">
         <v>381</v>
@@ -51809,7 +51809,7 @@
         <v>0.25</v>
       </c>
       <c r="R110" t="s">
-        <v>7185</v>
+        <v>7161</v>
       </c>
       <c r="S110" t="s">
         <v>381</v>
@@ -51824,7 +51824,7 @@
         <v>0.15</v>
       </c>
       <c r="W110" s="3" t="s">
-        <v>7199</v>
+        <v>7175</v>
       </c>
       <c r="AA110">
         <v>0.3</v>
@@ -51857,7 +51857,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="111" spans="1:72">
+    <row r="111" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>683</v>
       </c>
@@ -51880,7 +51880,7 @@
         <v>1018</v>
       </c>
       <c r="H111" t="s">
-        <v>7185</v>
+        <v>7161</v>
       </c>
       <c r="I111" t="s">
         <v>381</v>
@@ -51910,7 +51910,7 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="R111" t="s">
-        <v>7185</v>
+        <v>7161</v>
       </c>
       <c r="S111" t="s">
         <v>381</v>
@@ -51925,7 +51925,7 @@
         <v>0.125</v>
       </c>
       <c r="W111" s="3" t="s">
-        <v>7198</v>
+        <v>7174</v>
       </c>
       <c r="Y111" t="s">
         <v>381</v>
@@ -51937,7 +51937,7 @@
         <v>0.16250000000000001</v>
       </c>
       <c r="AB111" s="3" t="s">
-        <v>7200</v>
+        <v>7176</v>
       </c>
       <c r="AF111">
         <v>0.21249999999999999</v>
@@ -51967,7 +51967,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="112" spans="1:72">
+    <row r="112" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>500</v>
       </c>
@@ -51987,7 +51987,7 @@
         <v>381</v>
       </c>
       <c r="H112" t="s">
-        <v>7185</v>
+        <v>7161</v>
       </c>
       <c r="I112" t="s">
         <v>381</v>
@@ -52017,7 +52017,7 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="R112" t="s">
-        <v>7185</v>
+        <v>7161</v>
       </c>
       <c r="S112" t="s">
         <v>381</v>
@@ -52032,7 +52032,7 @@
         <v>0.125</v>
       </c>
       <c r="W112" s="3" t="s">
-        <v>7199</v>
+        <v>7175</v>
       </c>
       <c r="Y112" t="s">
         <v>381</v>
@@ -52044,7 +52044,7 @@
         <v>0.16250000000000001</v>
       </c>
       <c r="AB112" s="3" t="s">
-        <v>7201</v>
+        <v>7177</v>
       </c>
       <c r="AF112">
         <v>0.21249999999999999</v>
@@ -52074,7 +52074,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="113" spans="1:72">
+    <row r="113" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>684</v>
       </c>
@@ -52112,7 +52112,7 @@
         <v>0.4</v>
       </c>
       <c r="M113" t="s">
-        <v>7191</v>
+        <v>7167</v>
       </c>
       <c r="Q113">
         <v>0.1</v>
@@ -52124,7 +52124,7 @@
         <v>0.4</v>
       </c>
       <c r="W113" t="s">
-        <v>7191</v>
+        <v>7167</v>
       </c>
       <c r="AA113">
         <v>0.1</v>
@@ -52157,7 +52157,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="114" spans="1:72">
+    <row r="114" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>685</v>
       </c>
@@ -52180,7 +52180,7 @@
         <v>1020</v>
       </c>
       <c r="H114" t="s">
-        <v>7202</v>
+        <v>7178</v>
       </c>
       <c r="I114" t="s">
         <v>381</v>
@@ -52210,7 +52210,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="R114" t="s">
-        <v>7193</v>
+        <v>7169</v>
       </c>
       <c r="S114" t="s">
         <v>381</v>
@@ -52300,7 +52300,7 @@
         <v>0.125</v>
       </c>
       <c r="AV114" t="s">
-        <v>7193</v>
+        <v>7169</v>
       </c>
       <c r="AW114" t="s">
         <v>381</v>
@@ -52330,7 +52330,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="115" spans="1:72">
+    <row r="115" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>686</v>
       </c>
@@ -52353,7 +52353,7 @@
         <v>1021</v>
       </c>
       <c r="H115" t="s">
-        <v>7202</v>
+        <v>7178</v>
       </c>
       <c r="I115" t="s">
         <v>381</v>
@@ -52383,7 +52383,7 @@
         <v>0.1</v>
       </c>
       <c r="R115" t="s">
-        <v>7193</v>
+        <v>7169</v>
       </c>
       <c r="S115" t="s">
         <v>381</v>
@@ -52443,7 +52443,7 @@
         <v>0.15</v>
       </c>
       <c r="AL115" t="s">
-        <v>7193</v>
+        <v>7169</v>
       </c>
       <c r="AM115" t="s">
         <v>381</v>
@@ -52479,7 +52479,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="116" spans="1:72">
+    <row r="116" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>687</v>
       </c>
@@ -52556,7 +52556,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="117" spans="1:72">
+    <row r="117" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>688</v>
       </c>
@@ -52681,7 +52681,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="118" spans="1:72">
+    <row r="118" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>689</v>
       </c>
@@ -52755,7 +52755,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="119" spans="1:72">
+    <row r="119" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>506</v>
       </c>
@@ -52829,7 +52829,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="120" spans="1:72">
+    <row r="120" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>690</v>
       </c>
@@ -52906,7 +52906,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="121" spans="1:72">
+    <row r="121" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>507</v>
       </c>
@@ -52980,7 +52980,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="122" spans="1:72">
+    <row r="122" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>691</v>
       </c>
@@ -53057,7 +53057,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="123" spans="1:72">
+    <row r="123" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>508</v>
       </c>
@@ -53131,7 +53131,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="124" spans="1:72">
+    <row r="124" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>692</v>
       </c>
@@ -53184,7 +53184,7 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="R124" t="s">
-        <v>7185</v>
+        <v>7161</v>
       </c>
       <c r="S124" t="s">
         <v>381</v>
@@ -53199,7 +53199,7 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="W124" t="s">
-        <v>7197</v>
+        <v>7173</v>
       </c>
       <c r="AA124">
         <v>0.17499999999999999</v>
@@ -53232,7 +53232,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="125" spans="1:72">
+    <row r="125" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>693</v>
       </c>
@@ -53309,7 +53309,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="126" spans="1:72">
+    <row r="126" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>510</v>
       </c>
@@ -53383,7 +53383,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="127" spans="1:72">
+    <row r="127" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>694</v>
       </c>
@@ -53472,7 +53472,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="128" spans="1:72">
+    <row r="128" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>511</v>
       </c>
@@ -53558,7 +53558,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="129" spans="1:72">
+    <row r="129" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>695</v>
       </c>
@@ -53692,7 +53692,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="130" spans="1:72">
+    <row r="130" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>512</v>
       </c>
@@ -53763,7 +53763,7 @@
         <v>0.17499999999999996</v>
       </c>
     </row>
-    <row r="131" spans="1:72">
+    <row r="131" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>696</v>
       </c>
@@ -53888,7 +53888,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="132" spans="1:72">
+    <row r="132" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>697</v>
       </c>
@@ -53965,7 +53965,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="133" spans="1:72">
+    <row r="133" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>514</v>
       </c>
@@ -54039,7 +54039,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="134" spans="1:72">
+    <row r="134" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>698</v>
       </c>
@@ -54077,7 +54077,7 @@
         <v>0.4</v>
       </c>
       <c r="M134" t="s">
-        <v>7191</v>
+        <v>7167</v>
       </c>
       <c r="Q134">
         <v>0.1</v>
@@ -54089,7 +54089,7 @@
         <v>0.4</v>
       </c>
       <c r="W134" t="s">
-        <v>7191</v>
+        <v>7167</v>
       </c>
       <c r="AA134">
         <v>0.1</v>
@@ -54122,7 +54122,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="135" spans="1:72">
+    <row r="135" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>515</v>
       </c>
@@ -54157,7 +54157,7 @@
         <v>0.4</v>
       </c>
       <c r="M135" t="s">
-        <v>7191</v>
+        <v>7167</v>
       </c>
       <c r="Q135">
         <v>0.1</v>
@@ -54169,7 +54169,7 @@
         <v>0.4</v>
       </c>
       <c r="W135" t="s">
-        <v>7191</v>
+        <v>7167</v>
       </c>
       <c r="AA135">
         <v>0.1</v>
@@ -54202,7 +54202,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="136" spans="1:72">
+    <row r="136" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>699</v>
       </c>
@@ -54369,7 +54369,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="137" spans="1:72">
+    <row r="137" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>700</v>
       </c>
@@ -54536,7 +54536,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="138" spans="1:72">
+    <row r="138" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>701</v>
       </c>
@@ -54559,7 +54559,7 @@
         <v>1036</v>
       </c>
       <c r="H138" t="s">
-        <v>7202</v>
+        <v>7178</v>
       </c>
       <c r="I138" t="s">
         <v>381</v>
@@ -54589,7 +54589,7 @@
         <v>6.8250000000000005E-2</v>
       </c>
       <c r="R138" t="s">
-        <v>7193</v>
+        <v>7169</v>
       </c>
       <c r="S138" t="s">
         <v>381</v>
@@ -54709,7 +54709,7 @@
         <v>0.11375</v>
       </c>
       <c r="BF138" t="s">
-        <v>7193</v>
+        <v>7169</v>
       </c>
       <c r="BG138" t="s">
         <v>381</v>
@@ -54733,7 +54733,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="139" spans="1:72">
+    <row r="139" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>702</v>
       </c>
@@ -54810,7 +54810,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="140" spans="1:72">
+    <row r="140" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>703</v>
       </c>
@@ -54833,7 +54833,7 @@
         <v>1038</v>
       </c>
       <c r="H140" t="s">
-        <v>7185</v>
+        <v>7161</v>
       </c>
       <c r="I140" t="s">
         <v>381</v>
@@ -54977,7 +54977,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="141" spans="1:72">
+    <row r="141" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>704</v>
       </c>
@@ -55054,7 +55054,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="142" spans="1:72">
+    <row r="142" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>705</v>
       </c>
@@ -55131,7 +55131,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="143" spans="1:72">
+    <row r="143" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>706</v>
       </c>
@@ -55208,7 +55208,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="144" spans="1:72">
+    <row r="144" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>707</v>
       </c>
@@ -55285,7 +55285,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="145" spans="1:82">
+    <row r="145" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>708</v>
       </c>
@@ -55362,7 +55362,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="146" spans="1:82">
+    <row r="146" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>709</v>
       </c>
@@ -55439,7 +55439,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="147" spans="1:82">
+    <row r="147" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>710</v>
       </c>
@@ -55564,7 +55564,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="148" spans="1:82">
+    <row r="148" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>711</v>
       </c>
@@ -55731,7 +55731,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="149" spans="1:82">
+    <row r="149" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>712</v>
       </c>
@@ -55898,7 +55898,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="150" spans="1:82">
+    <row r="150" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>713</v>
       </c>
@@ -56065,12 +56065,12 @@
         <v>381</v>
       </c>
     </row>
-    <row r="151" spans="1:82">
+    <row r="151" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>7209</v>
+        <v>7183</v>
       </c>
       <c r="B151" t="s">
-        <v>7203</v>
+        <v>7179</v>
       </c>
       <c r="C151">
         <v>13</v>
@@ -56082,7 +56082,7 @@
         <v>536</v>
       </c>
       <c r="G151" t="s">
-        <v>7208</v>
+        <v>7182</v>
       </c>
       <c r="H151" t="s">
         <v>170</v>
@@ -56310,12 +56310,12 @@
         <v>381</v>
       </c>
     </row>
-    <row r="152" spans="1:82">
+    <row r="152" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>7210</v>
+        <v>7184</v>
       </c>
       <c r="B152" t="s">
-        <v>7204</v>
+        <v>7180</v>
       </c>
       <c r="C152">
         <v>10</v>
@@ -56327,7 +56327,7 @@
         <v>536</v>
       </c>
       <c r="G152" t="s">
-        <v>7207</v>
+        <v>7181</v>
       </c>
       <c r="H152" t="s">
         <v>170</v>
@@ -56556,7 +56556,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:DC150"/>
+  <autoFilter ref="A2:DC150" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="20">
     <mergeCell ref="CT1:CX1"/>
     <mergeCell ref="CY1:DC1"/>
@@ -57643,7 +57643,7 @@
         <v>0.21</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>7196</v>
+        <v>7172</v>
       </c>
       <c r="M30">
         <v>0.21</v>
@@ -57675,7 +57675,7 @@
         <v>0.21</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>7196</v>
+        <v>7172</v>
       </c>
       <c r="M31">
         <v>0.21</v>
@@ -57961,7 +57961,7 @@
         <v>0.33300000000000002</v>
       </c>
       <c r="H42" t="s">
-        <v>7179</v>
+        <v>7155</v>
       </c>
       <c r="I42">
         <v>0.66700000000000004</v>
@@ -57987,7 +57987,7 @@
         <v>0.3</v>
       </c>
       <c r="H43" t="s">
-        <v>7181</v>
+        <v>7157</v>
       </c>
       <c r="I43">
         <v>0.2</v>
@@ -58013,7 +58013,7 @@
         <v>0.3</v>
       </c>
       <c r="H44" t="s">
-        <v>7182</v>
+        <v>7158</v>
       </c>
       <c r="I44">
         <v>0.2</v>
@@ -58508,21 +58508,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DE52F0-FA25-3147-9398-011447F75847}">
   <dimension ref="A1:I158"/>
   <sheetViews>
-    <sheetView topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="A157" sqref="A157"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="C159" sqref="C159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col bestFit="true" customWidth="true" max="1" min="1" width="25.375"/>
-    <col bestFit="true" customWidth="true" max="2" min="2" width="41.125"/>
-    <col bestFit="true" customWidth="true" max="4" min="4" width="16.875"/>
-    <col customWidth="true" max="7" min="7" width="20.875"/>
-    <col customWidth="true" max="8" min="8" width="23.125"/>
-    <col bestFit="true" customWidth="true" max="23" min="23" width="120.625"/>
+    <col min="1" max="1" width="25.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.875" customWidth="1"/>
+    <col min="8" max="8" width="23.125" customWidth="1"/>
+    <col min="23" max="23" width="120.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -58539,7 +58539,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>765</v>
       </c>
@@ -58559,7 +58559,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>766</v>
       </c>
@@ -58579,7 +58579,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>767</v>
       </c>
@@ -58599,7 +58599,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>768</v>
       </c>
@@ -58619,7 +58619,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>769</v>
       </c>
@@ -58639,7 +58639,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>770</v>
       </c>
@@ -58659,7 +58659,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>771</v>
       </c>
@@ -58679,7 +58679,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>772</v>
       </c>
@@ -58699,7 +58699,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>773</v>
       </c>
@@ -58719,7 +58719,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>774</v>
       </c>
@@ -58739,7 +58739,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>775</v>
       </c>
@@ -58759,7 +58759,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>776</v>
       </c>
@@ -58779,7 +58779,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>777</v>
       </c>
@@ -58799,7 +58799,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>778</v>
       </c>
@@ -58819,7 +58819,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>779</v>
       </c>
@@ -58839,7 +58839,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>780</v>
       </c>
@@ -58859,7 +58859,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>781</v>
       </c>
@@ -58879,7 +58879,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>782</v>
       </c>
@@ -58899,7 +58899,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>783</v>
       </c>
@@ -58919,7 +58919,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>784</v>
       </c>
@@ -58939,7 +58939,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>785</v>
       </c>
@@ -58959,7 +58959,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>786</v>
       </c>
@@ -58979,7 +58979,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>787</v>
       </c>
@@ -58999,7 +58999,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>788</v>
       </c>
@@ -59019,7 +59019,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>789</v>
       </c>
@@ -59039,7 +59039,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>790</v>
       </c>
@@ -59059,7 +59059,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>791</v>
       </c>
@@ -59079,7 +59079,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>792</v>
       </c>
@@ -59099,7 +59099,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>793</v>
       </c>
@@ -59119,7 +59119,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>794</v>
       </c>
@@ -59139,7 +59139,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>795</v>
       </c>
@@ -59159,7 +59159,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>796</v>
       </c>
@@ -59179,7 +59179,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>797</v>
       </c>
@@ -59199,7 +59199,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>798</v>
       </c>
@@ -59219,7 +59219,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>799</v>
       </c>
@@ -59239,7 +59239,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>800</v>
       </c>
@@ -59259,7 +59259,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>801</v>
       </c>
@@ -59279,7 +59279,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>802</v>
       </c>
@@ -59299,7 +59299,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>803</v>
       </c>
@@ -59319,7 +59319,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>804</v>
       </c>
@@ -59339,7 +59339,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>805</v>
       </c>
@@ -59359,7 +59359,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>806</v>
       </c>
@@ -59379,7 +59379,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>807</v>
       </c>
@@ -59399,7 +59399,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>808</v>
       </c>
@@ -59419,7 +59419,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>809</v>
       </c>
@@ -59439,7 +59439,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>810</v>
       </c>
@@ -59459,7 +59459,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>811</v>
       </c>
@@ -59479,7 +59479,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>812</v>
       </c>
@@ -59499,7 +59499,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>813</v>
       </c>
@@ -59519,7 +59519,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>814</v>
       </c>
@@ -59539,7 +59539,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>815</v>
       </c>
@@ -59559,7 +59559,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>816</v>
       </c>
@@ -59579,7 +59579,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>817</v>
       </c>
@@ -59587,7 +59587,7 @@
         <v>428</v>
       </c>
       <c r="C54" t="s">
-        <v>7178</v>
+        <v>7154</v>
       </c>
       <c r="D54" t="s">
         <v>609</v>
@@ -59599,7 +59599,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>818</v>
       </c>
@@ -59619,7 +59619,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>819</v>
       </c>
@@ -59639,7 +59639,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>820</v>
       </c>
@@ -59659,7 +59659,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>821</v>
       </c>
@@ -59679,7 +59679,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>822</v>
       </c>
@@ -59699,7 +59699,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>823</v>
       </c>
@@ -59719,7 +59719,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>824</v>
       </c>
@@ -59739,7 +59739,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>825</v>
       </c>
@@ -59759,7 +59759,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>826</v>
       </c>
@@ -59779,7 +59779,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>827</v>
       </c>
@@ -59799,7 +59799,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>828</v>
       </c>
@@ -59819,7 +59819,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>829</v>
       </c>
@@ -59839,7 +59839,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>830</v>
       </c>
@@ -59859,7 +59859,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>831</v>
       </c>
@@ -59879,7 +59879,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>832</v>
       </c>
@@ -59899,7 +59899,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>833</v>
       </c>
@@ -59919,7 +59919,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>834</v>
       </c>
@@ -59939,7 +59939,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>835</v>
       </c>
@@ -59959,7 +59959,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>836</v>
       </c>
@@ -59979,7 +59979,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>837</v>
       </c>
@@ -59999,7 +59999,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>838</v>
       </c>
@@ -60019,7 +60019,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>839</v>
       </c>
@@ -60039,7 +60039,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>840</v>
       </c>
@@ -60059,7 +60059,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>841</v>
       </c>
@@ -60079,7 +60079,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>842</v>
       </c>
@@ -60099,7 +60099,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>843</v>
       </c>
@@ -60119,7 +60119,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>844</v>
       </c>
@@ -60139,7 +60139,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>845</v>
       </c>
@@ -60159,7 +60159,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>846</v>
       </c>
@@ -60179,7 +60179,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>847</v>
       </c>
@@ -60199,7 +60199,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>848</v>
       </c>
@@ -60219,7 +60219,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>849</v>
       </c>
@@ -60239,7 +60239,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>850</v>
       </c>
@@ -60259,7 +60259,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>851</v>
       </c>
@@ -60279,7 +60279,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>852</v>
       </c>
@@ -60299,7 +60299,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>853</v>
       </c>
@@ -60319,7 +60319,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>854</v>
       </c>
@@ -60339,7 +60339,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>855</v>
       </c>
@@ -60359,7 +60359,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>856</v>
       </c>
@@ -60379,7 +60379,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>857</v>
       </c>
@@ -60399,7 +60399,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>858</v>
       </c>
@@ -60419,7 +60419,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>859</v>
       </c>
@@ -60439,7 +60439,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>860</v>
       </c>
@@ -60447,7 +60447,7 @@
         <v>471</v>
       </c>
       <c r="C97" t="s">
-        <v>7118</v>
+        <v>7187</v>
       </c>
       <c r="D97" t="s">
         <v>609</v>
@@ -60459,7 +60459,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>861</v>
       </c>
@@ -60467,7 +60467,7 @@
         <v>472</v>
       </c>
       <c r="C98" t="s">
-        <v>7119</v>
+        <v>7188</v>
       </c>
       <c r="D98" t="s">
         <v>609</v>
@@ -60479,7 +60479,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>862</v>
       </c>
@@ -60487,7 +60487,7 @@
         <v>473</v>
       </c>
       <c r="C99" t="s">
-        <v>7120</v>
+        <v>7189</v>
       </c>
       <c r="D99" t="s">
         <v>609</v>
@@ -60499,7 +60499,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>863</v>
       </c>
@@ -60507,7 +60507,7 @@
         <v>474</v>
       </c>
       <c r="C100" t="s">
-        <v>7121</v>
+        <v>7190</v>
       </c>
       <c r="D100" t="s">
         <v>609</v>
@@ -60519,7 +60519,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>864</v>
       </c>
@@ -60527,7 +60527,7 @@
         <v>475</v>
       </c>
       <c r="C101" t="s">
-        <v>7122</v>
+        <v>7191</v>
       </c>
       <c r="D101" t="s">
         <v>609</v>
@@ -60539,7 +60539,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>865</v>
       </c>
@@ -60547,7 +60547,7 @@
         <v>476</v>
       </c>
       <c r="C102" t="s">
-        <v>7123</v>
+        <v>7192</v>
       </c>
       <c r="D102" t="s">
         <v>609</v>
@@ -60559,7 +60559,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>866</v>
       </c>
@@ -60567,7 +60567,7 @@
         <v>477</v>
       </c>
       <c r="C103" t="s">
-        <v>7124</v>
+        <v>7193</v>
       </c>
       <c r="D103" t="s">
         <v>609</v>
@@ -60579,7 +60579,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>867</v>
       </c>
@@ -60587,7 +60587,7 @@
         <v>478</v>
       </c>
       <c r="C104" t="s">
-        <v>7125</v>
+        <v>7194</v>
       </c>
       <c r="D104" t="s">
         <v>609</v>
@@ -60599,7 +60599,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>868</v>
       </c>
@@ -60607,7 +60607,7 @@
         <v>479</v>
       </c>
       <c r="C105" t="s">
-        <v>7126</v>
+        <v>7195</v>
       </c>
       <c r="D105" t="s">
         <v>609</v>
@@ -60619,7 +60619,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>869</v>
       </c>
@@ -60627,7 +60627,7 @@
         <v>480</v>
       </c>
       <c r="C106" t="s">
-        <v>7127</v>
+        <v>7196</v>
       </c>
       <c r="D106" t="s">
         <v>609</v>
@@ -60639,7 +60639,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>870</v>
       </c>
@@ -60647,7 +60647,7 @@
         <v>481</v>
       </c>
       <c r="C107" t="s">
-        <v>7128</v>
+        <v>7197</v>
       </c>
       <c r="D107" t="s">
         <v>609</v>
@@ -60659,7 +60659,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>871</v>
       </c>
@@ -60667,7 +60667,7 @@
         <v>482</v>
       </c>
       <c r="C108" t="s">
-        <v>7129</v>
+        <v>7118</v>
       </c>
       <c r="D108" t="s">
         <v>609</v>
@@ -60679,7 +60679,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>872</v>
       </c>
@@ -60687,7 +60687,7 @@
         <v>483</v>
       </c>
       <c r="C109" t="s">
-        <v>7130</v>
+        <v>7119</v>
       </c>
       <c r="D109" t="s">
         <v>609</v>
@@ -60699,7 +60699,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>873</v>
       </c>
@@ -60707,7 +60707,7 @@
         <v>484</v>
       </c>
       <c r="C110" t="s">
-        <v>7131</v>
+        <v>7198</v>
       </c>
       <c r="D110" t="s">
         <v>609</v>
@@ -60719,7 +60719,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>874</v>
       </c>
@@ -60727,7 +60727,7 @@
         <v>485</v>
       </c>
       <c r="C111" t="s">
-        <v>7132</v>
+        <v>7120</v>
       </c>
       <c r="D111" t="s">
         <v>609</v>
@@ -60739,7 +60739,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>875</v>
       </c>
@@ -60747,7 +60747,7 @@
         <v>486</v>
       </c>
       <c r="C112" t="s">
-        <v>7133</v>
+        <v>7121</v>
       </c>
       <c r="D112" t="s">
         <v>609</v>
@@ -60759,7 +60759,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="113" spans="1:9">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>876</v>
       </c>
@@ -60767,7 +60767,7 @@
         <v>487</v>
       </c>
       <c r="C113" t="s">
-        <v>7134</v>
+        <v>7122</v>
       </c>
       <c r="D113" t="s">
         <v>609</v>
@@ -60779,7 +60779,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>877</v>
       </c>
@@ -60787,7 +60787,7 @@
         <v>488</v>
       </c>
       <c r="C114" t="s">
-        <v>7135</v>
+        <v>7123</v>
       </c>
       <c r="D114" t="s">
         <v>609</v>
@@ -60799,7 +60799,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>878</v>
       </c>
@@ -60807,7 +60807,7 @@
         <v>489</v>
       </c>
       <c r="C115" t="s">
-        <v>7136</v>
+        <v>7124</v>
       </c>
       <c r="D115" t="s">
         <v>609</v>
@@ -60819,7 +60819,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>879</v>
       </c>
@@ -60827,7 +60827,7 @@
         <v>490</v>
       </c>
       <c r="C116" t="s">
-        <v>7137</v>
+        <v>7125</v>
       </c>
       <c r="D116" t="s">
         <v>609</v>
@@ -60839,7 +60839,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>880</v>
       </c>
@@ -60847,7 +60847,7 @@
         <v>491</v>
       </c>
       <c r="C117" t="s">
-        <v>7138</v>
+        <v>7126</v>
       </c>
       <c r="D117" t="s">
         <v>609</v>
@@ -60859,7 +60859,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>881</v>
       </c>
@@ -60867,7 +60867,7 @@
         <v>492</v>
       </c>
       <c r="C118" t="s">
-        <v>7139</v>
+        <v>7127</v>
       </c>
       <c r="D118" t="s">
         <v>609</v>
@@ -60879,7 +60879,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>882</v>
       </c>
@@ -60887,7 +60887,7 @@
         <v>493</v>
       </c>
       <c r="C119" t="s">
-        <v>7140</v>
+        <v>7128</v>
       </c>
       <c r="D119" t="s">
         <v>609</v>
@@ -60899,7 +60899,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="120" spans="1:9">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>883</v>
       </c>
@@ -60907,7 +60907,7 @@
         <v>494</v>
       </c>
       <c r="C120" t="s">
-        <v>7141</v>
+        <v>7129</v>
       </c>
       <c r="D120" t="s">
         <v>609</v>
@@ -60919,7 +60919,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>884</v>
       </c>
@@ -60927,7 +60927,7 @@
         <v>495</v>
       </c>
       <c r="C121" t="s">
-        <v>7142</v>
+        <v>7130</v>
       </c>
       <c r="D121" t="s">
         <v>609</v>
@@ -60939,7 +60939,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="122" spans="1:9">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>885</v>
       </c>
@@ -60947,7 +60947,7 @@
         <v>496</v>
       </c>
       <c r="C122" t="s">
-        <v>7143</v>
+        <v>7131</v>
       </c>
       <c r="D122" t="s">
         <v>609</v>
@@ -60959,7 +60959,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>886</v>
       </c>
@@ -60967,7 +60967,7 @@
         <v>497</v>
       </c>
       <c r="C123" t="s">
-        <v>7144</v>
+        <v>7132</v>
       </c>
       <c r="D123" t="s">
         <v>609</v>
@@ -60979,7 +60979,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="124" spans="1:9">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>887</v>
       </c>
@@ -60987,7 +60987,7 @@
         <v>498</v>
       </c>
       <c r="C124" t="s">
-        <v>7145</v>
+        <v>7133</v>
       </c>
       <c r="D124" t="s">
         <v>609</v>
@@ -60999,7 +60999,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="125" spans="1:9">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>888</v>
       </c>
@@ -61007,7 +61007,7 @@
         <v>499</v>
       </c>
       <c r="C125" t="s">
-        <v>7146</v>
+        <v>7134</v>
       </c>
       <c r="D125" t="s">
         <v>609</v>
@@ -61019,7 +61019,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="126" spans="1:9">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>889</v>
       </c>
@@ -61027,7 +61027,7 @@
         <v>500</v>
       </c>
       <c r="C126" t="s">
-        <v>7147</v>
+        <v>7135</v>
       </c>
       <c r="D126" t="s">
         <v>609</v>
@@ -61039,7 +61039,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="127" spans="1:9">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>890</v>
       </c>
@@ -61047,7 +61047,7 @@
         <v>501</v>
       </c>
       <c r="C127" t="s">
-        <v>7148</v>
+        <v>7136</v>
       </c>
       <c r="D127" t="s">
         <v>609</v>
@@ -61059,7 +61059,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="128" spans="1:9">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>891</v>
       </c>
@@ -61067,7 +61067,7 @@
         <v>502</v>
       </c>
       <c r="C128" t="s">
-        <v>7149</v>
+        <v>7199</v>
       </c>
       <c r="D128" t="s">
         <v>609</v>
@@ -61079,7 +61079,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>892</v>
       </c>
@@ -61087,7 +61087,7 @@
         <v>503</v>
       </c>
       <c r="C129" t="s">
-        <v>7150</v>
+        <v>7137</v>
       </c>
       <c r="D129" t="s">
         <v>609</v>
@@ -61099,7 +61099,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="130" spans="1:9">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>893</v>
       </c>
@@ -61107,7 +61107,7 @@
         <v>504</v>
       </c>
       <c r="C130" t="s">
-        <v>7151</v>
+        <v>7138</v>
       </c>
       <c r="D130" t="s">
         <v>609</v>
@@ -61119,7 +61119,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>894</v>
       </c>
@@ -61127,7 +61127,7 @@
         <v>505</v>
       </c>
       <c r="C131" t="s">
-        <v>7152</v>
+        <v>7200</v>
       </c>
       <c r="D131" t="s">
         <v>609</v>
@@ -61139,7 +61139,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="132" spans="1:9">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>895</v>
       </c>
@@ -61147,7 +61147,7 @@
         <v>506</v>
       </c>
       <c r="C132" t="s">
-        <v>7153</v>
+        <v>7139</v>
       </c>
       <c r="D132" t="s">
         <v>609</v>
@@ -61159,7 +61159,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>896</v>
       </c>
@@ -61167,7 +61167,7 @@
         <v>507</v>
       </c>
       <c r="C133" t="s">
-        <v>7154</v>
+        <v>7140</v>
       </c>
       <c r="D133" t="s">
         <v>609</v>
@@ -61179,7 +61179,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>897</v>
       </c>
@@ -61187,7 +61187,7 @@
         <v>508</v>
       </c>
       <c r="C134" t="s">
-        <v>7155</v>
+        <v>7201</v>
       </c>
       <c r="D134" t="s">
         <v>609</v>
@@ -61199,7 +61199,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>898</v>
       </c>
@@ -61207,7 +61207,7 @@
         <v>509</v>
       </c>
       <c r="C135" t="s">
-        <v>7156</v>
+        <v>7141</v>
       </c>
       <c r="D135" t="s">
         <v>609</v>
@@ -61219,7 +61219,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="136" spans="1:9">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>899</v>
       </c>
@@ -61227,7 +61227,7 @@
         <v>510</v>
       </c>
       <c r="C136" t="s">
-        <v>7157</v>
+        <v>7142</v>
       </c>
       <c r="D136" t="s">
         <v>609</v>
@@ -61239,7 +61239,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>900</v>
       </c>
@@ -61247,7 +61247,7 @@
         <v>511</v>
       </c>
       <c r="C137" t="s">
-        <v>7158</v>
+        <v>7143</v>
       </c>
       <c r="D137" t="s">
         <v>609</v>
@@ -61259,7 +61259,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="138" spans="1:9">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>901</v>
       </c>
@@ -61267,7 +61267,7 @@
         <v>512</v>
       </c>
       <c r="C138" t="s">
-        <v>7159</v>
+        <v>7144</v>
       </c>
       <c r="D138" t="s">
         <v>609</v>
@@ -61279,7 +61279,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>902</v>
       </c>
@@ -61287,7 +61287,7 @@
         <v>513</v>
       </c>
       <c r="C139" t="s">
-        <v>7160</v>
+        <v>7145</v>
       </c>
       <c r="D139" t="s">
         <v>609</v>
@@ -61299,7 +61299,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="140" spans="1:9">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>903</v>
       </c>
@@ -61307,7 +61307,7 @@
         <v>514</v>
       </c>
       <c r="C140" t="s">
-        <v>7161</v>
+        <v>7146</v>
       </c>
       <c r="D140" t="s">
         <v>609</v>
@@ -61319,7 +61319,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="141" spans="1:9">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>904</v>
       </c>
@@ -61327,7 +61327,7 @@
         <v>515</v>
       </c>
       <c r="C141" t="s">
-        <v>7162</v>
+        <v>7147</v>
       </c>
       <c r="D141" t="s">
         <v>609</v>
@@ -61339,7 +61339,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>905</v>
       </c>
@@ -61347,7 +61347,7 @@
         <v>516</v>
       </c>
       <c r="C142" t="s">
-        <v>7163</v>
+        <v>7148</v>
       </c>
       <c r="D142" t="s">
         <v>609</v>
@@ -61359,7 +61359,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="143" spans="1:9">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>906</v>
       </c>
@@ -61367,7 +61367,7 @@
         <v>517</v>
       </c>
       <c r="C143" t="s">
-        <v>7164</v>
+        <v>7149</v>
       </c>
       <c r="D143" t="s">
         <v>609</v>
@@ -61379,7 +61379,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="144" spans="1:9">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>907</v>
       </c>
@@ -61387,7 +61387,7 @@
         <v>518</v>
       </c>
       <c r="C144" t="s">
-        <v>7165</v>
+        <v>7202</v>
       </c>
       <c r="D144" t="s">
         <v>609</v>
@@ -61399,7 +61399,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="145" spans="1:9">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>908</v>
       </c>
@@ -61407,7 +61407,7 @@
         <v>519</v>
       </c>
       <c r="C145" t="s">
-        <v>7166</v>
+        <v>7203</v>
       </c>
       <c r="D145" t="s">
         <v>609</v>
@@ -61419,7 +61419,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="146" spans="1:9">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>909</v>
       </c>
@@ -61427,7 +61427,7 @@
         <v>520</v>
       </c>
       <c r="C146" t="s">
-        <v>7167</v>
+        <v>7150</v>
       </c>
       <c r="D146" t="s">
         <v>609</v>
@@ -61439,7 +61439,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>910</v>
       </c>
@@ -61447,7 +61447,7 @@
         <v>521</v>
       </c>
       <c r="C147" t="s">
-        <v>7168</v>
+        <v>7204</v>
       </c>
       <c r="D147" t="s">
         <v>609</v>
@@ -61459,7 +61459,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="148" spans="1:9">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>911</v>
       </c>
@@ -61467,7 +61467,7 @@
         <v>522</v>
       </c>
       <c r="C148" t="s">
-        <v>7169</v>
+        <v>7205</v>
       </c>
       <c r="D148" t="s">
         <v>609</v>
@@ -61479,7 +61479,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="149" spans="1:9">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>912</v>
       </c>
@@ -61487,7 +61487,7 @@
         <v>523</v>
       </c>
       <c r="C149" t="s">
-        <v>7170</v>
+        <v>7206</v>
       </c>
       <c r="D149" t="s">
         <v>609</v>
@@ -61499,7 +61499,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="150" spans="1:9">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>913</v>
       </c>
@@ -61507,7 +61507,7 @@
         <v>524</v>
       </c>
       <c r="C150" t="s">
-        <v>7171</v>
+        <v>7207</v>
       </c>
       <c r="D150" t="s">
         <v>609</v>
@@ -61519,7 +61519,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="151" spans="1:9">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>914</v>
       </c>
@@ -61527,7 +61527,7 @@
         <v>525</v>
       </c>
       <c r="C151" t="s">
-        <v>7172</v>
+        <v>7208</v>
       </c>
       <c r="D151" t="s">
         <v>609</v>
@@ -61539,7 +61539,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="152" spans="1:9">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>915</v>
       </c>
@@ -61547,7 +61547,7 @@
         <v>526</v>
       </c>
       <c r="C152" t="s">
-        <v>7173</v>
+        <v>7209</v>
       </c>
       <c r="D152" t="s">
         <v>609</v>
@@ -61559,7 +61559,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="153" spans="1:9">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>916</v>
       </c>
@@ -61567,7 +61567,7 @@
         <v>527</v>
       </c>
       <c r="C153" t="s">
-        <v>7174</v>
+        <v>7210</v>
       </c>
       <c r="D153" t="s">
         <v>609</v>
@@ -61579,7 +61579,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="154" spans="1:9">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>917</v>
       </c>
@@ -61587,7 +61587,7 @@
         <v>528</v>
       </c>
       <c r="C154" t="s">
-        <v>7175</v>
+        <v>7151</v>
       </c>
       <c r="D154" t="s">
         <v>609</v>
@@ -61599,7 +61599,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="155" spans="1:9">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>918</v>
       </c>
@@ -61607,7 +61607,7 @@
         <v>529</v>
       </c>
       <c r="C155" t="s">
-        <v>7176</v>
+        <v>7152</v>
       </c>
       <c r="D155" t="s">
         <v>609</v>
@@ -61619,7 +61619,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="156" spans="1:9">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>919</v>
       </c>
@@ -61627,7 +61627,7 @@
         <v>530</v>
       </c>
       <c r="C156" t="s">
-        <v>7177</v>
+        <v>7153</v>
       </c>
       <c r="D156" t="s">
         <v>609</v>
@@ -61639,15 +61639,15 @@
         <v>554</v>
       </c>
     </row>
-    <row r="157" spans="1:9">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
+        <v>7185</v>
+      </c>
+      <c r="B157" t="s">
+        <v>7179</v>
+      </c>
+      <c r="C157" t="s">
         <v>7211</v>
-      </c>
-      <c r="B157" t="s">
-        <v>7203</v>
-      </c>
-      <c r="C157" t="s">
-        <v>7206</v>
       </c>
       <c r="D157" t="s">
         <v>609</v>
@@ -61656,15 +61656,15 @@
         <v>6.875</v>
       </c>
     </row>
-    <row r="158" spans="1:9">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
+        <v>7186</v>
+      </c>
+      <c r="B158" t="s">
+        <v>7180</v>
+      </c>
+      <c r="C158" t="s">
         <v>7212</v>
-      </c>
-      <c r="B158" t="s">
-        <v>7204</v>
-      </c>
-      <c r="C158" t="s">
-        <v>7205</v>
       </c>
       <c r="D158" t="s">
         <v>609</v>

</xml_diff>

<commit_message>
finished all imgs for now
</commit_message>
<xml_diff>
--- a/assets/posesaxl.xlsx
+++ b/assets/posesaxl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jam/go/i9posesa/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DCA70F-381C-AF41-99CA-B2A87C686B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF31B9F-F88B-2746-85B0-FADD4E80F9C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ImageSets" sheetId="1" r:id="rId1"/>
@@ -22195,8 +22195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0C6FEDB-7242-034A-A2CD-5F1C567957CE}">
   <dimension ref="A1:AA274"/>
   <sheetViews>
-    <sheetView topLeftCell="A242" workbookViewId="0">
-      <selection activeCell="B275" sqref="B275"/>
+    <sheetView tabSelected="1" topLeftCell="A242" workbookViewId="0">
+      <selection activeCell="C243" sqref="C243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -41774,7 +41774,7 @@
       </c>
     </row>
     <row r="266" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B266" t="s">
+      <c r="B266" s="3" t="s">
         <v>7224</v>
       </c>
       <c r="C266" t="str">
@@ -41783,7 +41783,7 @@
       </c>
     </row>
     <row r="267" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B267" t="s">
+      <c r="B267" s="3" t="s">
         <v>7225</v>
       </c>
       <c r="C267" t="str">
@@ -41792,7 +41792,7 @@
       </c>
     </row>
     <row r="268" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B268" t="s">
+      <c r="B268" s="3" t="s">
         <v>7222</v>
       </c>
       <c r="C268" t="str">
@@ -41801,7 +41801,7 @@
       </c>
     </row>
     <row r="269" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B269" t="s">
+      <c r="B269" s="3" t="s">
         <v>7223</v>
       </c>
       <c r="C269" t="str">
@@ -41810,7 +41810,7 @@
       </c>
     </row>
     <row r="270" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B270" t="s">
+      <c r="B270" s="3" t="s">
         <v>7220</v>
       </c>
       <c r="C270" t="str">
@@ -41819,7 +41819,7 @@
       </c>
     </row>
     <row r="271" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B271" t="s">
+      <c r="B271" s="3" t="s">
         <v>7221</v>
       </c>
       <c r="C271" t="str">
@@ -41828,7 +41828,7 @@
       </c>
     </row>
     <row r="272" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B272" t="s">
+      <c r="B272" s="3" t="s">
         <v>7226</v>
       </c>
       <c r="C272" t="str">
@@ -41837,7 +41837,7 @@
       </c>
     </row>
     <row r="273" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B273" t="s">
+      <c r="B273" s="3" t="s">
         <v>7227</v>
       </c>
       <c r="C273" t="str">
@@ -41846,7 +41846,7 @@
       </c>
     </row>
     <row r="274" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B274" t="s">
+      <c r="B274" s="3" t="s">
         <v>7217</v>
       </c>
       <c r="C274" t="str">
@@ -41867,8 +41867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B5179E-762C-124B-A240-3A035CE5971A}">
   <dimension ref="A1:DC152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C67" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C91" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="F91" sqref="F91"/>
@@ -56769,14 +56769,6 @@
   </sheetData>
   <autoFilter ref="A2:DC150" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="20">
-    <mergeCell ref="CT1:CX1"/>
-    <mergeCell ref="CY1:DC1"/>
-    <mergeCell ref="BP1:BT1"/>
-    <mergeCell ref="BU1:BY1"/>
-    <mergeCell ref="BZ1:CD1"/>
-    <mergeCell ref="CE1:CI1"/>
-    <mergeCell ref="CJ1:CN1"/>
-    <mergeCell ref="CO1:CS1"/>
     <mergeCell ref="BK1:BO1"/>
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="M1:Q1"/>
@@ -56789,6 +56781,14 @@
     <mergeCell ref="AV1:AZ1"/>
     <mergeCell ref="BA1:BE1"/>
     <mergeCell ref="BF1:BJ1"/>
+    <mergeCell ref="CT1:CX1"/>
+    <mergeCell ref="CY1:DC1"/>
+    <mergeCell ref="BP1:BT1"/>
+    <mergeCell ref="BU1:BY1"/>
+    <mergeCell ref="BZ1:CD1"/>
+    <mergeCell ref="CE1:CI1"/>
+    <mergeCell ref="CJ1:CN1"/>
+    <mergeCell ref="CO1:CS1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -56798,8 +56798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899AC92B-5D4B-8E46-9E29-8D79D673E29D}">
   <dimension ref="A1:BC50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="E19" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -58421,6 +58421,20 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AP1:AQ1"/>
+    <mergeCell ref="AR1:AS1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
     <mergeCell ref="AV1:AW1"/>
     <mergeCell ref="AX1:AY1"/>
     <mergeCell ref="AZ1:BA1"/>
@@ -58432,20 +58446,6 @@
     <mergeCell ref="AJ1:AK1"/>
     <mergeCell ref="AL1:AM1"/>
     <mergeCell ref="AT1:AU1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="AP1:AQ1"/>
-    <mergeCell ref="AR1:AS1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
tweaked shoudler tap plank
</commit_message>
<xml_diff>
--- a/assets/posesaxl.xlsx
+++ b/assets/posesaxl.xlsx
@@ -8,9 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jam/go/i9posesa/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF31B9F-F88B-2746-85B0-FADD4E80F9C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ImageSets" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <sheet name="Transitions" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Exercises!$A$2:$DC$150</definedName>
+    <definedName hidden="true" localSheetId="1" name="_xlnm._FilterDatabase">Exercises!$A$2:$DC$150</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12872" uniqueCount="7256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12871" uniqueCount="7256">
   <si>
     <t>ID</t>
   </si>
@@ -21817,8 +21816,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -21862,10 +21861,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -21884,7 +21883,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -21897,7 +21896,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -22195,7 +22194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0C6FEDB-7242-034A-A2CD-5F1C567957CE}">
   <dimension ref="A1:AA274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A242" workbookViewId="0">
+    <sheetView topLeftCell="A242" workbookViewId="0">
       <selection activeCell="C243" sqref="C243"/>
     </sheetView>
   </sheetViews>
@@ -41867,11 +41866,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B5179E-762C-124B-A240-3A035CE5971A}">
   <dimension ref="A1:DC152"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C91" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C111" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F91" sqref="F91"/>
+      <selection pane="bottomRight" activeCell="F138" sqref="F138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -54258,16 +54257,13 @@
         <v>515</v>
       </c>
       <c r="C134">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D134">
-        <v>0.25</v>
+        <v>0.67</v>
       </c>
       <c r="E134" t="s">
         <v>538</v>
-      </c>
-      <c r="F134" t="s">
-        <v>381</v>
       </c>
       <c r="G134" t="s">
         <v>1033</v>
@@ -56769,6 +56765,14 @@
   </sheetData>
   <autoFilter ref="A2:DC150" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="20">
+    <mergeCell ref="CT1:CX1"/>
+    <mergeCell ref="CY1:DC1"/>
+    <mergeCell ref="BP1:BT1"/>
+    <mergeCell ref="BU1:BY1"/>
+    <mergeCell ref="BZ1:CD1"/>
+    <mergeCell ref="CE1:CI1"/>
+    <mergeCell ref="CJ1:CN1"/>
+    <mergeCell ref="CO1:CS1"/>
     <mergeCell ref="BK1:BO1"/>
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="M1:Q1"/>
@@ -56781,14 +56785,6 @@
     <mergeCell ref="AV1:AZ1"/>
     <mergeCell ref="BA1:BE1"/>
     <mergeCell ref="BF1:BJ1"/>
-    <mergeCell ref="CT1:CX1"/>
-    <mergeCell ref="CY1:DC1"/>
-    <mergeCell ref="BP1:BT1"/>
-    <mergeCell ref="BU1:BY1"/>
-    <mergeCell ref="BZ1:CD1"/>
-    <mergeCell ref="CE1:CI1"/>
-    <mergeCell ref="CJ1:CN1"/>
-    <mergeCell ref="CO1:CS1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -58421,20 +58417,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="AP1:AQ1"/>
-    <mergeCell ref="AR1:AS1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:O1"/>
     <mergeCell ref="AV1:AW1"/>
     <mergeCell ref="AX1:AY1"/>
     <mergeCell ref="AZ1:BA1"/>
@@ -58446,6 +58428,20 @@
     <mergeCell ref="AJ1:AK1"/>
     <mergeCell ref="AL1:AM1"/>
     <mergeCell ref="AT1:AU1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AP1:AQ1"/>
+    <mergeCell ref="AR1:AS1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -58964,8 +58960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DE52F0-FA25-3147-9398-011447F75847}">
   <dimension ref="A1:I165"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+    <sheetView topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="E141" sqref="E141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>